<commit_message>
JPY: new synth depo and new calendar rule
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/JPY/JPY_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/JPY/JPY_YCSTDBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15225" yWindow="-15" windowWidth="15270" windowHeight="7680" tabRatio="726" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="15240" windowHeight="8055" tabRatio="726" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="Accuracy">'General Settings'!$D$19</definedName>
     <definedName name="BondBasisDayCounter">'General Settings'!$M$13</definedName>
-    <definedName name="Calendar">'General Settings'!$D$18</definedName>
+    <definedName name="Calendar">'General Settings'!$M$24</definedName>
     <definedName name="Conventions" localSheetId="6">Swaps!$O$5:$Q$9</definedName>
     <definedName name="Currency">'General Settings'!$D$4</definedName>
     <definedName name="DepoInclusionCriteria">Selected!$B$5</definedName>
@@ -29,9 +29,13 @@
     <definedName name="FileOverwrite">'General Settings'!$M$6</definedName>
     <definedName name="FrontFuturesRollingDays">Selected!$B$4</definedName>
     <definedName name="GENERAL_SETTINGS">'General Settings'!$K$9</definedName>
+    <definedName name="HolidayCheck">'General Settings'!$M$21</definedName>
     <definedName name="IborType">'General Settings'!$D$7</definedName>
     <definedName name="IndexTenor">'General Settings'!$D$6</definedName>
     <definedName name="InterpolatorID">'General Settings'!$D$21</definedName>
+    <definedName name="JoinCalendar">'General Settings'!$M$23</definedName>
+    <definedName name="LiborCalendar">'General Settings'!$M$20</definedName>
+    <definedName name="LocalCalendar">'General Settings'!$M$19</definedName>
     <definedName name="MinDistance">RateHelpers!$K$2:$K$99</definedName>
     <definedName name="MoneyMarketDayCounter">'General Settings'!$M$14</definedName>
     <definedName name="Months">'General Settings'!$D$5</definedName>
@@ -48,7 +52,6 @@
     <definedName name="RateHelpersSelected">Selected!$A$7</definedName>
     <definedName name="SerializationPath">'General Settings'!$M$5</definedName>
     <definedName name="Serialize">'General Settings'!$M$4</definedName>
-    <definedName name="SwapCalendar">'General Settings'!$M$22</definedName>
     <definedName name="SwapFixedFreq">'General Settings'!$D$8</definedName>
     <definedName name="TraitsID">'General Settings'!$D$20</definedName>
     <definedName name="Trigger">'General Settings'!$D$11</definedName>
@@ -220,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="145">
   <si>
     <t>60Y</t>
   </si>
@@ -636,22 +639,25 @@
     <t>CALENDAR SETTINGS</t>
   </si>
   <si>
-    <t>Calendar 1</t>
-  </si>
-  <si>
-    <t>Calendar 2</t>
-  </si>
-  <si>
     <t>Join Calendar Rule</t>
-  </si>
-  <si>
-    <t>Swap Calendar</t>
   </si>
   <si>
     <t>JoinHolidays</t>
   </si>
   <si>
     <t>UnitedKingdom::Exchange</t>
+  </si>
+  <si>
+    <t>JPY Calendar</t>
+  </si>
+  <si>
+    <t>Libor Calendar</t>
+  </si>
+  <si>
+    <t>HolidayCheck</t>
+  </si>
+  <si>
+    <t>Join Calendar</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1336,7 @@
     <xf numFmtId="175" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="175" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1784,6 +1790,22 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="2" fillId="4" borderId="10" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="2" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="2" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="4"/>
@@ -2179,7 +2201,7 @@
     <row r="1" spans="1:33" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.5.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Nov 18 2014 09:26:00</v>
+        <v>QuantLibXL 1.5.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Dec 24 2014 09:17:06</v>
       </c>
     </row>
     <row r="2" spans="1:33" s="3" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2541,9 +2563,7 @@
       <c r="C11" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="25">
-        <v>41996.382222222222</v>
-      </c>
+      <c r="D11" s="25"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="28"/>
@@ -2668,7 +2688,7 @@
       </c>
       <c r="D14" s="22" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,_xll.ohPack(Selected!D2:D126),,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_JPYYCSTD#0005</v>
+        <v>_JPYYCSTD#0003</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -2788,7 +2808,7 @@
       <c r="AF16" s="3"/>
       <c r="AG16" s="3"/>
     </row>
-    <row r="17" spans="1:33" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="5"/>
       <c r="C17" s="14" t="s">
@@ -2827,7 +2847,7 @@
       <c r="AF17" s="3"/>
       <c r="AG17" s="3"/>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="5"/>
       <c r="C18" s="14" t="s">
@@ -2842,10 +2862,10 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="105"/>
-      <c r="L18" s="106"/>
-      <c r="M18" s="106"/>
-      <c r="N18" s="107"/>
+      <c r="K18" s="199"/>
+      <c r="L18" s="200"/>
+      <c r="M18" s="200"/>
+      <c r="N18" s="201"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
@@ -2882,14 +2902,14 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="M19" s="36" t="s">
+      <c r="K19" s="199"/>
+      <c r="L19" s="202" t="s">
+        <v>141</v>
+      </c>
+      <c r="M19" s="203" t="s">
         <v>124</v>
       </c>
-      <c r="N19" s="32"/>
+      <c r="N19" s="201"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
@@ -2925,14 +2945,14 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="M20" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="N20" s="32"/>
+      <c r="K20" s="199"/>
+      <c r="L20" s="202" t="s">
+        <v>142</v>
+      </c>
+      <c r="M20" s="204" t="s">
+        <v>140</v>
+      </c>
+      <c r="N20" s="201"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
@@ -2968,14 +2988,15 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="M21" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="N21" s="32"/>
+      <c r="K21" s="199"/>
+      <c r="L21" s="202" t="s">
+        <v>143</v>
+      </c>
+      <c r="M21" s="204" t="b">
+        <f>_xll.qlCalendarIsHoliday(LocalCalendar,_xll.qlCalendarAdvance(LiborCalendar,_xll.qlSettingsEvaluationDate(Trigger),2&amp;"D","f",FALSE,Trigger))</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="201"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
@@ -3007,15 +3028,14 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="69"/>
-      <c r="L22" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="M22" s="36" t="str">
-        <f>M21&amp;"("&amp;M19&amp;","&amp;M20&amp;")"</f>
-        <v>JoinHolidays(Japan,UnitedKingdom::Exchange)</v>
-      </c>
-      <c r="N22" s="68"/>
+      <c r="K22" s="199"/>
+      <c r="L22" s="202" t="s">
+        <v>138</v>
+      </c>
+      <c r="M22" s="205" t="s">
+        <v>139</v>
+      </c>
+      <c r="N22" s="201"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
@@ -3036,16 +3056,16 @@
       <c r="AF22" s="3"/>
       <c r="AG22" s="3"/>
     </row>
-    <row r="23" spans="1:33" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
       <c r="C23" s="9">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41997</v>
+        <v>42032</v>
       </c>
       <c r="D23" s="8">
         <f>MAX(_xll.ohPack(Selected!J1:J126))</f>
-        <v>1.4556954057314556E-2</v>
+        <v>1.3636110672599748E-2</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -3053,10 +3073,15 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="37"/>
+      <c r="K23" s="199"/>
+      <c r="L23" s="202" t="s">
+        <v>144</v>
+      </c>
+      <c r="M23" s="205" t="str">
+        <f>M22&amp;"("&amp;LocalCalendar&amp;","&amp;LiborCalendar&amp;")"</f>
+        <v>JoinHolidays(Japan,UnitedKingdom::Exchange)</v>
+      </c>
+      <c r="N23" s="201"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
@@ -3077,16 +3102,16 @@
       <c r="AF23" s="3"/>
       <c r="AG23" s="3"/>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
       <c r="C24" s="7">
         <f>MAX(_xll.ohPack(Selected!I2:I126))</f>
-        <v>52961</v>
+        <v>52992</v>
       </c>
       <c r="D24" s="6">
         <f>MIN(_xll.ohPack(Selected!J1:J126))</f>
-        <v>5.3593891239512345E-4</v>
+        <v>4.1275253303319951E-4</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -3094,10 +3119,15 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
+      <c r="K24" s="199"/>
+      <c r="L24" s="202" t="s">
+        <v>64</v>
+      </c>
+      <c r="M24" s="205" t="str">
+        <f>IF(HolidayCheck,JoinCalendar,LiborCalendar)</f>
+        <v>UnitedKingdom::Exchange</v>
+      </c>
+      <c r="N24" s="201"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
@@ -3118,7 +3148,7 @@
       <c r="AF24" s="3"/>
       <c r="AG24" s="3"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="5"/>
       <c r="C25" s="70" t="s">
@@ -3134,10 +3164,10 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
+      <c r="K25" s="206"/>
+      <c r="L25" s="207"/>
+      <c r="M25" s="207"/>
+      <c r="N25" s="208"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -4564,11 +4594,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M13:M14">
       <formula1>"Actual/Actual (ISDA),Actual/360,30/360 (Bond Basis),30E/360 (Eurobond Basis),Actual/365 (Fixed),Actual/Actual (ISMA),Actual/Actual (AFB),1/1,30/360 (Italian),Simple"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M19 M20">
-      <formula1>"TARGET,UnitedKingdom::Exchange,UnitedKingdom::Metals,UnitedKingdom::Settlement,UnitedStates::GovernmentBond,UnitedStates::NERC,UnitedStates::NYSE,UnitedStates::Settlement,Switzerland,Japan,Italy::Exchange,NullCalendar,Australia,China,HongKong::HKEx"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M22">
+      <formula1>"JoinBusinessDays,JoinHolidays"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M21">
-      <formula1>"JoinBusinessDays,JoinHolidays"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M19:M20">
+      <formula1>"TARGET,UnitedKingdom::Exchange,UnitedKingdom::Metals,UnitedKingdom::Settlement,UnitedStates::GovernmentBond,UnitedStates::NERC,UnitedStates::NYSE,UnitedStates::Settlement,Switzerland,Japan,Italy::Exchange,NullCalendar"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4648,7 +4678,7 @@
       </c>
       <c r="E2" s="117" t="str">
         <f>Deposits!E3</f>
-        <v>obj_0032a#0000</v>
+        <v>obj_0034e#0002</v>
       </c>
       <c r="F2" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E2),"LastFixing","D"),"Libor","")</f>
@@ -4670,11 +4700,11 @@
       </c>
       <c r="L2" s="119">
         <f>_xll.qlRateHelperEarliestDate($E2,Trigger)</f>
-        <v>41997</v>
+        <v>42032</v>
       </c>
       <c r="M2" s="120">
         <f>_xll.qlRateHelperLatestDate($E2,Trigger)</f>
-        <v>41998</v>
+        <v>42033</v>
       </c>
       <c r="N2" s="63">
         <v>10</v>
@@ -4691,7 +4721,7 @@
       </c>
       <c r="E3" s="117" t="str">
         <f>Deposits!E4</f>
-        <v>obj_00328#0000</v>
+        <v>obj_0034d#0002</v>
       </c>
       <c r="F3" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E3),"LastFixing","D"),"Libor","")</f>
@@ -4699,7 +4729,7 @@
       </c>
       <c r="G3" s="118">
         <f>_xll.qlRateHelperQuoteValue($E3,Trigger)</f>
-        <v>4.2860000000000001E-4</v>
+        <v>3.3570000000000003E-4</v>
       </c>
       <c r="H3" s="118"/>
       <c r="I3" s="65" t="b">
@@ -4713,11 +4743,11 @@
       </c>
       <c r="L3" s="119">
         <f>_xll.qlRateHelperEarliestDate($E3,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M3" s="120">
         <f>_xll.qlRateHelperLatestDate($E3,Trigger)</f>
-        <v>42009</v>
+        <v>42037</v>
       </c>
       <c r="N3" s="63">
         <v>20</v>
@@ -4734,7 +4764,7 @@
       </c>
       <c r="E4" s="117" t="str">
         <f>Deposits!E5</f>
-        <v>obj_00320#0000</v>
+        <v>obj_00319#0002</v>
       </c>
       <c r="F4" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E4),"LastFixing","D"),"Libor","")</f>
@@ -4742,7 +4772,7 @@
       </c>
       <c r="G4" s="118">
         <f>_xll.qlRateHelperQuoteValue($E4,Trigger)</f>
-        <v>5.2859999999999995E-4</v>
+        <v>4.0709999999999997E-4</v>
       </c>
       <c r="H4" s="118"/>
       <c r="I4" s="65" t="b">
@@ -4756,11 +4786,11 @@
       </c>
       <c r="L4" s="119">
         <f>_xll.qlRateHelperEarliestDate($E4,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M4" s="120">
         <f>_xll.qlRateHelperLatestDate($E4,Trigger)</f>
-        <v>42010</v>
+        <v>42041</v>
       </c>
       <c r="N4" s="63">
         <v>30</v>
@@ -4777,7 +4807,7 @@
       </c>
       <c r="E5" s="117" t="str">
         <f>Deposits!E8</f>
-        <v>obj_00326#0000</v>
+        <v>obj_00327#0002</v>
       </c>
       <c r="F5" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E5),"LastFixing","D"),"Libor","")</f>
@@ -4785,7 +4815,7 @@
       </c>
       <c r="G5" s="118">
         <f>_xll.qlRateHelperQuoteValue($E5,Trigger)</f>
-        <v>8.5000000000000006E-4</v>
+        <v>7.1429999999999996E-4</v>
       </c>
       <c r="H5" s="118"/>
       <c r="I5" s="65" t="b">
@@ -4799,11 +4829,11 @@
       </c>
       <c r="L5" s="119">
         <f>_xll.qlRateHelperEarliestDate($E5,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M5" s="120">
         <f>_xll.qlRateHelperLatestDate($E5,Trigger)</f>
-        <v>42034</v>
+        <v>42062</v>
       </c>
       <c r="N5" s="63">
         <v>60</v>
@@ -4820,7 +4850,7 @@
       </c>
       <c r="E6" s="117" t="str">
         <f>Deposits!E9</f>
-        <v>obj_0031c#0000</v>
+        <v>obj_00320#0002</v>
       </c>
       <c r="F6" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E6),"LastFixing","D"),"Libor","")</f>
@@ -4828,7 +4858,7 @@
       </c>
       <c r="G6" s="118">
         <f>_xll.qlRateHelperQuoteValue($E6,Trigger)</f>
-        <v>1.0571000000000001E-3</v>
+        <v>9.0709999999999999E-4</v>
       </c>
       <c r="H6" s="118"/>
       <c r="I6" s="65" t="b">
@@ -4842,11 +4872,11 @@
       </c>
       <c r="L6" s="119">
         <f>_xll.qlRateHelperEarliestDate($E6,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M6" s="120">
         <f>_xll.qlRateHelperLatestDate($E6,Trigger)</f>
-        <v>42062</v>
+        <v>42094</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4857,7 +4887,7 @@
       </c>
       <c r="E7" s="117" t="str">
         <f>Deposits!E10</f>
-        <v>obj_00322#0000</v>
+        <v>obj_0031d#0002</v>
       </c>
       <c r="F7" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E7),"LastFixing","D"),"Libor","")</f>
@@ -4865,7 +4895,7 @@
       </c>
       <c r="G7" s="118">
         <f>_xll.qlRateHelperQuoteValue($E7,Trigger)</f>
-        <v>1.1286E-3</v>
+        <v>1.0214E-3</v>
       </c>
       <c r="H7" s="118"/>
       <c r="I7" s="65" t="b">
@@ -4879,11 +4909,11 @@
       </c>
       <c r="L7" s="119">
         <f>_xll.qlRateHelperEarliestDate($E7,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M7" s="120">
         <f>_xll.qlRateHelperLatestDate($E7,Trigger)</f>
-        <v>42093</v>
+        <v>42124</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4894,7 +4924,7 @@
       </c>
       <c r="E8" s="117" t="str">
         <f>Deposits!E13</f>
-        <v>obj_00325#0000</v>
+        <v>obj_00324#0002</v>
       </c>
       <c r="F8" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E8),"LastFixing","D"),"Libor","")</f>
@@ -4902,7 +4932,7 @@
       </c>
       <c r="G8" s="118">
         <f>_xll.qlRateHelperQuoteValue($E8,Trigger)</f>
-        <v>1.6286E-3</v>
+        <v>1.4357E-3</v>
       </c>
       <c r="H8" s="118"/>
       <c r="I8" s="65" t="b">
@@ -4916,11 +4946,11 @@
       </c>
       <c r="L8" s="119">
         <f>_xll.qlRateHelperEarliestDate($E8,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M8" s="120">
         <f>_xll.qlRateHelperLatestDate($E8,Trigger)</f>
-        <v>42185</v>
+        <v>42216</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4931,7 +4961,7 @@
       </c>
       <c r="E9" s="117" t="str">
         <f>Deposits!E19</f>
-        <v>obj_00317#0000</v>
+        <v>obj_00315#0002</v>
       </c>
       <c r="F9" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E9),"LastFixing","D"),"Libor","")</f>
@@ -4939,7 +4969,7 @@
       </c>
       <c r="G9" s="118">
         <f>_xll.qlRateHelperQuoteValue($E9,Trigger)</f>
-        <v>3.2042999999999998E-3</v>
+        <v>2.6756999999999996E-3</v>
       </c>
       <c r="H9" s="118"/>
       <c r="I9" s="65" t="b">
@@ -4953,11 +4983,11 @@
       </c>
       <c r="L9" s="119">
         <f>_xll.qlRateHelperEarliestDate($E9,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M9" s="120">
         <f>_xll.qlRateHelperLatestDate($E9,Trigger)</f>
-        <v>42368</v>
+        <v>42398</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4973,7 +5003,7 @@
       </c>
       <c r="E10" s="133" t="str">
         <f>FRAs!G3</f>
-        <v>obj_0031d#0000</v>
+        <v>obj_00323#0002</v>
       </c>
       <c r="F10" s="133" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E10),"LastFixing","D"),"Libor","")</f>
@@ -4981,7 +5011,7 @@
       </c>
       <c r="G10" s="134">
         <f>_xll.qlRateHelperQuoteValue($E10,Trigger)</f>
-        <v>1.15E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="H10" s="134"/>
       <c r="I10" s="135" t="b">
@@ -4995,11 +5025,11 @@
       </c>
       <c r="L10" s="136">
         <f>_xll.qlRateHelperEarliestDate($E10,Trigger)</f>
-        <v>42034</v>
+        <v>42062</v>
       </c>
       <c r="M10" s="137">
         <f>_xll.qlRateHelperLatestDate($E10,Trigger)</f>
-        <v>42124</v>
+        <v>42153</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5015,7 +5045,7 @@
       </c>
       <c r="E11" s="117" t="str">
         <f>FRAs!G4</f>
-        <v>obj_00321#0000</v>
+        <v>obj_0031b#0002</v>
       </c>
       <c r="F11" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E11),"LastFixing","D"),"Libor","")</f>
@@ -5023,7 +5053,7 @@
       </c>
       <c r="G11" s="118">
         <f>_xll.qlRateHelperQuoteValue($E11,Trigger)</f>
-        <v>1.15E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="H11" s="118"/>
       <c r="I11" s="65" t="b">
@@ -5037,11 +5067,11 @@
       </c>
       <c r="L11" s="119">
         <f>_xll.qlRateHelperEarliestDate($E11,Trigger)</f>
-        <v>42062</v>
+        <v>42094</v>
       </c>
       <c r="M11" s="120">
         <f>_xll.qlRateHelperLatestDate($E11,Trigger)</f>
-        <v>42153</v>
+        <v>42185</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5057,7 +5087,7 @@
       </c>
       <c r="E12" s="117" t="str">
         <f>FRAs!G5</f>
-        <v>obj_00318#0000</v>
+        <v>obj_00318#0002</v>
       </c>
       <c r="F12" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E12),"LastFixing","D"),"Libor","")</f>
@@ -5065,7 +5095,7 @@
       </c>
       <c r="G12" s="118">
         <f>_xll.qlRateHelperQuoteValue($E12,Trigger)</f>
-        <v>1.15E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="H12" s="118"/>
       <c r="I12" s="65" t="b">
@@ -5079,11 +5109,11 @@
       </c>
       <c r="L12" s="119">
         <f>_xll.qlRateHelperEarliestDate($E12,Trigger)</f>
-        <v>42093</v>
+        <v>42124</v>
       </c>
       <c r="M12" s="120">
         <f>_xll.qlRateHelperLatestDate($E12,Trigger)</f>
-        <v>42185</v>
+        <v>42216</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5099,7 +5129,7 @@
       </c>
       <c r="E13" s="117" t="str">
         <f>FRAs!G6</f>
-        <v>obj_0031e#0000</v>
+        <v>obj_00326#0002</v>
       </c>
       <c r="F13" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E13),"LastFixing","D"),"Libor","")</f>
@@ -5107,7 +5137,7 @@
       </c>
       <c r="G13" s="118">
         <f>_xll.qlRateHelperQuoteValue($E13,Trigger)</f>
-        <v>1.15E-3</v>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="H13" s="118"/>
       <c r="I13" s="65" t="b">
@@ -5121,11 +5151,11 @@
       </c>
       <c r="L13" s="119">
         <f>_xll.qlRateHelperEarliestDate($E13,Trigger)</f>
-        <v>42124</v>
+        <v>42153</v>
       </c>
       <c r="M13" s="120">
         <f>_xll.qlRateHelperLatestDate($E13,Trigger)</f>
-        <v>42216</v>
+        <v>42244</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5141,7 +5171,7 @@
       </c>
       <c r="E14" s="117" t="str">
         <f>FRAs!G7</f>
-        <v>obj_00316#0000</v>
+        <v>obj_00325#0002</v>
       </c>
       <c r="F14" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E14),"LastFixing","D"),"Libor","")</f>
@@ -5149,7 +5179,7 @@
       </c>
       <c r="G14" s="118">
         <f>_xll.qlRateHelperQuoteValue($E14,Trigger)</f>
-        <v>1.15E-3</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="H14" s="118"/>
       <c r="I14" s="65" t="b">
@@ -5163,11 +5193,11 @@
       </c>
       <c r="L14" s="119">
         <f>_xll.qlRateHelperEarliestDate($E14,Trigger)</f>
-        <v>42153</v>
+        <v>42185</v>
       </c>
       <c r="M14" s="120">
         <f>_xll.qlRateHelperLatestDate($E14,Trigger)</f>
-        <v>42244</v>
+        <v>42277</v>
       </c>
     </row>
     <row r="15" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5183,7 +5213,7 @@
       </c>
       <c r="E15" s="117" t="str">
         <f>FRAs!G8</f>
-        <v>obj_00324#0000</v>
+        <v>obj_00321#0002</v>
       </c>
       <c r="F15" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E15),"LastFixing","D"),"Libor","")</f>
@@ -5191,7 +5221,7 @@
       </c>
       <c r="G15" s="118">
         <f>_xll.qlRateHelperQuoteValue($E15,Trigger)</f>
-        <v>1.15E-3</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="H15" s="118"/>
       <c r="I15" s="65" t="b">
@@ -5205,11 +5235,11 @@
       </c>
       <c r="L15" s="119">
         <f>_xll.qlRateHelperEarliestDate($E15,Trigger)</f>
-        <v>42185</v>
+        <v>42216</v>
       </c>
       <c r="M15" s="120">
         <f>_xll.qlRateHelperLatestDate($E15,Trigger)</f>
-        <v>42277</v>
+        <v>42307</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5225,7 +5255,7 @@
       </c>
       <c r="E16" s="117" t="str">
         <f>FRAs!G9</f>
-        <v>obj_0031b#0000</v>
+        <v>obj_0031e#0002</v>
       </c>
       <c r="F16" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E16),"LastFixing","D"),"Libor","")</f>
@@ -5233,7 +5263,7 @@
       </c>
       <c r="G16" s="118">
         <f>_xll.qlRateHelperQuoteValue($E16,Trigger)</f>
-        <v>1.1000000000000001E-3</v>
+        <v>1.15E-3</v>
       </c>
       <c r="H16" s="118"/>
       <c r="I16" s="65" t="b">
@@ -5247,11 +5277,11 @@
       </c>
       <c r="L16" s="119">
         <f>_xll.qlRateHelperEarliestDate($E16,Trigger)</f>
-        <v>42277</v>
+        <v>42307</v>
       </c>
       <c r="M16" s="120">
         <f>_xll.qlRateHelperLatestDate($E16,Trigger)</f>
-        <v>42368</v>
+        <v>42398</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5267,7 +5297,7 @@
       </c>
       <c r="E17" s="117" t="str">
         <f>FRAs!G10</f>
-        <v>obj_00327#0000</v>
+        <v>obj_00317#0002</v>
       </c>
       <c r="F17" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E17),"LastFixing","D"),"Libor","")</f>
@@ -5289,11 +5319,11 @@
       </c>
       <c r="L17" s="119">
         <f>_xll.qlRateHelperEarliestDate($E17,Trigger)</f>
-        <v>42368</v>
+        <v>42398</v>
       </c>
       <c r="M17" s="120">
         <f>_xll.qlRateHelperLatestDate($E17,Trigger)</f>
-        <v>42460</v>
+        <v>42488</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5309,7 +5339,7 @@
       </c>
       <c r="E18" s="117" t="str">
         <f>FRAs!G11</f>
-        <v>obj_0031a#0000</v>
+        <v>obj_0031c#0002</v>
       </c>
       <c r="F18" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E18),"LastFixing","D"),"Libor","")</f>
@@ -5317,7 +5347,7 @@
       </c>
       <c r="G18" s="118">
         <f>_xll.qlRateHelperQuoteValue($E18,Trigger)</f>
-        <v>1.0500000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="H18" s="118"/>
       <c r="I18" s="65" t="b">
@@ -5331,11 +5361,11 @@
       </c>
       <c r="L18" s="119">
         <f>_xll.qlRateHelperEarliestDate($E18,Trigger)</f>
-        <v>42459</v>
+        <v>42489</v>
       </c>
       <c r="M18" s="120">
         <f>_xll.qlRateHelperLatestDate($E18,Trigger)</f>
-        <v>42551</v>
+        <v>42580</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5351,7 +5381,7 @@
       </c>
       <c r="E19" s="117" t="str">
         <f>FRAs!G12</f>
-        <v>obj_00315#0000</v>
+        <v>obj_00322#0002</v>
       </c>
       <c r="F19" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E19),"LastFixing","D"),"Libor","")</f>
@@ -5359,7 +5389,7 @@
       </c>
       <c r="G19" s="118">
         <f>_xll.qlRateHelperQuoteValue($E19,Trigger)</f>
-        <v>1.0500000000000002E-3</v>
+        <v>1.15E-3</v>
       </c>
       <c r="H19" s="118"/>
       <c r="I19" s="65" t="b">
@@ -5373,11 +5403,11 @@
       </c>
       <c r="L19" s="119">
         <f>_xll.qlRateHelperEarliestDate($E19,Trigger)</f>
-        <v>42551</v>
+        <v>42580</v>
       </c>
       <c r="M19" s="120">
         <f>_xll.qlRateHelperLatestDate($E19,Trigger)</f>
-        <v>42643</v>
+        <v>42674</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5393,7 +5423,7 @@
       </c>
       <c r="E20" s="122" t="str">
         <f>FRAs!G13</f>
-        <v>obj_00319#0000</v>
+        <v>obj_0031a#0002</v>
       </c>
       <c r="F20" s="122" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E20),"LastFixing","D"),"Libor","")</f>
@@ -5401,7 +5431,7 @@
       </c>
       <c r="G20" s="123">
         <f>_xll.qlRateHelperQuoteValue($E20,Trigger)</f>
-        <v>1.1000000000000001E-3</v>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="H20" s="123"/>
       <c r="I20" s="124" t="b">
@@ -5415,11 +5445,11 @@
       </c>
       <c r="L20" s="125">
         <f>_xll.qlRateHelperEarliestDate($E20,Trigger)</f>
-        <v>42643</v>
+        <v>42674</v>
       </c>
       <c r="M20" s="126">
         <f>_xll.qlRateHelperLatestDate($E20,Trigger)</f>
-        <v>42734</v>
+        <v>42766</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5433,15 +5463,15 @@
       </c>
       <c r="D21" s="117" t="str">
         <f t="array" ref="D21:D62">_xll.qlIMMNextCodes(_xll.qlSettingsEvaluationDate(Trigger)-1,$A21:$A62)</f>
-        <v>F5</v>
+        <v>G5</v>
       </c>
       <c r="E21" s="117" t="str">
         <f>Futures!H3</f>
-        <v>obj_00342#0000</v>
+        <v>obj_0036e#0002</v>
       </c>
       <c r="F21" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E21),"LastFixing","D"),"Libor","")</f>
-        <v>JPYFUT3MF5_Quote</v>
+        <v>JPYFUT3MG5_Quote</v>
       </c>
       <c r="G21" s="130" t="e">
         <f>_xll.qlRateHelperQuoteValue(E21,Trigger)</f>
@@ -5479,15 +5509,15 @@
         <v>FUT3M</v>
       </c>
       <c r="D22" s="117" t="str">
-        <v>G5</v>
+        <v>H5</v>
       </c>
       <c r="E22" s="117" t="str">
         <f>Futures!H4</f>
-        <v>obj_00365#0000</v>
+        <v>obj_00360#0002</v>
       </c>
       <c r="F22" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E22),"LastFixing","D"),"Libor","")</f>
-        <v>JPYFUT3MG5_Quote</v>
+        <v>JPYFUT3MH5_Quote</v>
       </c>
       <c r="G22" s="130" t="e">
         <f>_xll.qlRateHelperQuoteValue(E22,Trigger)</f>
@@ -5525,15 +5555,15 @@
         <v>FUT3M</v>
       </c>
       <c r="D23" s="117" t="str">
-        <v>H5</v>
+        <v>J5</v>
       </c>
       <c r="E23" s="117" t="str">
         <f>Futures!H5</f>
-        <v>obj_0035d#0000</v>
+        <v>obj_0036b#0002</v>
       </c>
       <c r="F23" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E23),"LastFixing","D"),"Libor","")</f>
-        <v>JPYFUT3MH5_Quote</v>
+        <v>JPYFUT3MJ5_Quote</v>
       </c>
       <c r="G23" s="130" t="e">
         <f>_xll.qlRateHelperQuoteValue(E23,Trigger)</f>
@@ -5571,15 +5601,15 @@
         <v>FUT3M</v>
       </c>
       <c r="D24" s="117" t="str">
-        <v>J5</v>
+        <v>K5</v>
       </c>
       <c r="E24" s="117" t="str">
         <f>Futures!H6</f>
-        <v>obj_0035c#0000</v>
+        <v>obj_00376#0002</v>
       </c>
       <c r="F24" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E24),"LastFixing","D"),"Libor","")</f>
-        <v>JPYFUT3MJ5_Quote</v>
+        <v>JPYFUT3MK5_Quote</v>
       </c>
       <c r="G24" s="130" t="e">
         <f>_xll.qlRateHelperQuoteValue(E24,Trigger)</f>
@@ -5617,15 +5647,15 @@
         <v>FUT3M</v>
       </c>
       <c r="D25" s="117" t="str">
-        <v>K5</v>
+        <v>M5</v>
       </c>
       <c r="E25" s="117" t="str">
         <f>Futures!H7</f>
-        <v>obj_0036d#0000</v>
+        <v>obj_00359#0002</v>
       </c>
       <c r="F25" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E25),"LastFixing","D"),"Libor","")</f>
-        <v>JPYFUT3MK5_Quote</v>
+        <v>JPYFUT3MM5_Quote</v>
       </c>
       <c r="G25" s="130" t="e">
         <f>_xll.qlRateHelperQuoteValue(E25,Trigger)</f>
@@ -5663,15 +5693,15 @@
         <v>FUT3M</v>
       </c>
       <c r="D26" s="117" t="str">
-        <v>M5</v>
+        <v>N5</v>
       </c>
       <c r="E26" s="117" t="str">
         <f>Futures!H8</f>
-        <v>obj_00348#0000</v>
+        <v>obj_00356#0002</v>
       </c>
       <c r="F26" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E26),"LastFixing","D"),"Libor","")</f>
-        <v>JPYFUT3MM5_Quote</v>
+        <v>JPYFUT3MN5_Quote</v>
       </c>
       <c r="G26" s="130" t="e">
         <f>_xll.qlRateHelperQuoteValue(E26,Trigger)</f>
@@ -5709,15 +5739,15 @@
         <v>FUT3M</v>
       </c>
       <c r="D27" s="117" t="str">
-        <v>N5</v>
+        <v>Q5</v>
       </c>
       <c r="E27" s="117" t="str">
         <f>Futures!H9</f>
-        <v>obj_00355#0000</v>
+        <v>obj_00372#0002</v>
       </c>
       <c r="F27" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E27),"LastFixing","D"),"Libor","")</f>
-        <v>JPYFUT3MN5_Quote</v>
+        <v>JPYFUT3MQ5_Quote</v>
       </c>
       <c r="G27" s="130" t="e">
         <f>_xll.qlRateHelperQuoteValue(E27,Trigger)</f>
@@ -5755,15 +5785,15 @@
         <v>FUT3M</v>
       </c>
       <c r="D28" s="117" t="str">
-        <v>Q5</v>
+        <v>U5</v>
       </c>
       <c r="E28" s="117" t="str">
         <f>Futures!H10</f>
-        <v>obj_00360#0000</v>
+        <v>obj_00358#0002</v>
       </c>
       <c r="F28" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E28),"LastFixing","D"),"Libor","")</f>
-        <v>JPYFUT3MQ5_Quote</v>
+        <v>JPYFUT3MU5_Quote</v>
       </c>
       <c r="G28" s="130" t="e">
         <f>_xll.qlRateHelperQuoteValue(E28,Trigger)</f>
@@ -5801,15 +5831,15 @@
         <v>FUT3M</v>
       </c>
       <c r="D29" s="117" t="str">
-        <v>U5</v>
+        <v>V5</v>
       </c>
       <c r="E29" s="117" t="str">
         <f>Futures!H11</f>
-        <v>obj_00376#0000</v>
+        <v>obj_0036c#0002</v>
       </c>
       <c r="F29" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E29),"LastFixing","D"),"Libor","")</f>
-        <v>JPYFUT3MU5_Quote</v>
+        <v>JPYFUT3MV5_Quote</v>
       </c>
       <c r="G29" s="130" t="e">
         <f>_xll.qlRateHelperQuoteValue(E29,Trigger)</f>
@@ -5847,15 +5877,15 @@
         <v>FUT3M</v>
       </c>
       <c r="D30" s="117" t="str">
-        <v>V5</v>
+        <v>X5</v>
       </c>
       <c r="E30" s="117" t="str">
         <f>Futures!H12</f>
-        <v>obj_00332#0000</v>
+        <v>obj_00364#0002</v>
       </c>
       <c r="F30" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E30),"LastFixing","D"),"Libor","")</f>
-        <v>JPYFUT3MV5_Quote</v>
+        <v>JPYFUT3MX5_Quote</v>
       </c>
       <c r="G30" s="130" t="e">
         <f>_xll.qlRateHelperQuoteValue(E30,Trigger)</f>
@@ -5893,15 +5923,15 @@
         <v>FUT3M</v>
       </c>
       <c r="D31" s="117" t="str">
-        <v>X5</v>
+        <v>Z5</v>
       </c>
       <c r="E31" s="117" t="str">
         <f>Futures!H13</f>
-        <v>obj_00346#0000</v>
+        <v>obj_0036a#0002</v>
       </c>
       <c r="F31" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E31),"LastFixing","D"),"Libor","")</f>
-        <v>JPYFUT3MX5_Quote</v>
+        <v>JPYFUT3MZ5_Quote</v>
       </c>
       <c r="G31" s="130" t="e">
         <f>_xll.qlRateHelperQuoteValue(E31,Trigger)</f>
@@ -5939,15 +5969,15 @@
         <v>FUT3M</v>
       </c>
       <c r="D32" s="117" t="str">
-        <v>Z5</v>
+        <v>F6</v>
       </c>
       <c r="E32" s="117" t="str">
         <f>Futures!H14</f>
-        <v>obj_0034a#0000</v>
+        <v>obj_0035f#0002</v>
       </c>
       <c r="F32" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E32),"LastFixing","D"),"Libor","")</f>
-        <v>JPYFUT3MZ5_Quote</v>
+        <v>JPYFUT3MF6_Quote</v>
       </c>
       <c r="G32" s="130" t="e">
         <f>_xll.qlRateHelperQuoteValue(E32,Trigger)</f>
@@ -5989,7 +6019,7 @@
       </c>
       <c r="E33" s="117" t="str">
         <f>Futures!H15</f>
-        <v>obj_00331#0000</v>
+        <v>obj_00361#0002</v>
       </c>
       <c r="F33" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E33),"LastFixing","D"),"Libor","")</f>
@@ -6035,7 +6065,7 @@
       </c>
       <c r="E34" s="117" t="str">
         <f>Futures!H16</f>
-        <v>obj_00340#0000</v>
+        <v>obj_0035b#0002</v>
       </c>
       <c r="F34" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E34),"LastFixing","D"),"Libor","")</f>
@@ -6081,7 +6111,7 @@
       </c>
       <c r="E35" s="117" t="str">
         <f>Futures!H17</f>
-        <v>obj_0032f#0000</v>
+        <v>obj_0035e#0002</v>
       </c>
       <c r="F35" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E35),"LastFixing","D"),"Libor","")</f>
@@ -6127,7 +6157,7 @@
       </c>
       <c r="E36" s="117" t="str">
         <f>Futures!H18</f>
-        <v>obj_00344#0000</v>
+        <v>obj_00374#0002</v>
       </c>
       <c r="F36" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E36),"LastFixing","D"),"Libor","")</f>
@@ -6173,7 +6203,7 @@
       </c>
       <c r="E37" s="117" t="str">
         <f>Futures!H19</f>
-        <v>obj_00349#0000</v>
+        <v>obj_0035c#0002</v>
       </c>
       <c r="F37" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E37),"LastFixing","D"),"Libor","")</f>
@@ -6219,7 +6249,7 @@
       </c>
       <c r="E38" s="117" t="str">
         <f>Futures!H20</f>
-        <v>obj_00378#0000</v>
+        <v>obj_0035a#0002</v>
       </c>
       <c r="F38" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E38),"LastFixing","D"),"Libor","")</f>
@@ -6265,7 +6295,7 @@
       </c>
       <c r="E39" s="117" t="str">
         <f>Futures!H21</f>
-        <v>obj_00377#0000</v>
+        <v>obj_00354#0002</v>
       </c>
       <c r="F39" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E39),"LastFixing","D"),"Libor","")</f>
@@ -6311,7 +6341,7 @@
       </c>
       <c r="E40" s="117" t="str">
         <f>Futures!H22</f>
-        <v>obj_0033f#0000</v>
+        <v>obj_00355#0002</v>
       </c>
       <c r="F40" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E40),"LastFixing","D"),"Libor","")</f>
@@ -6357,7 +6387,7 @@
       </c>
       <c r="E41" s="117" t="str">
         <f>Futures!H23</f>
-        <v>obj_0035e#0000</v>
+        <v>obj_00352#0002</v>
       </c>
       <c r="F41" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E41),"LastFixing","D"),"Libor","")</f>
@@ -6403,7 +6433,7 @@
       </c>
       <c r="E42" s="117" t="str">
         <f>Futures!H24</f>
-        <v>obj_00368#0000</v>
+        <v>obj_00366#0002</v>
       </c>
       <c r="F42" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E42),"LastFixing","D"),"Libor","")</f>
@@ -6449,7 +6479,7 @@
       </c>
       <c r="E43" s="117" t="str">
         <f>Futures!H25</f>
-        <v>obj_00351#0000</v>
+        <v>obj_00377#0002</v>
       </c>
       <c r="F43" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E43),"LastFixing","D"),"Libor","")</f>
@@ -6495,7 +6525,7 @@
       </c>
       <c r="E44" s="117" t="str">
         <f>Futures!H26</f>
-        <v>obj_00336#0000</v>
+        <v>obj_00375#0002</v>
       </c>
       <c r="F44" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E44),"LastFixing","D"),"Libor","")</f>
@@ -6541,7 +6571,7 @@
       </c>
       <c r="E45" s="117" t="str">
         <f>Futures!H27</f>
-        <v>obj_00362#0000</v>
+        <v>obj_0036d#0002</v>
       </c>
       <c r="F45" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E45),"LastFixing","D"),"Libor","")</f>
@@ -6587,7 +6617,7 @@
       </c>
       <c r="E46" s="117" t="str">
         <f>Futures!H28</f>
-        <v>obj_0034e#0000</v>
+        <v>obj_00365#0002</v>
       </c>
       <c r="F46" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E46),"LastFixing","D"),"Libor","")</f>
@@ -6633,7 +6663,7 @@
       </c>
       <c r="E47" s="117" t="str">
         <f>Futures!H29</f>
-        <v>obj_0034c#0000</v>
+        <v>obj_00362#0002</v>
       </c>
       <c r="F47" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E47),"LastFixing","D"),"Libor","")</f>
@@ -6679,7 +6709,7 @@
       </c>
       <c r="E48" s="117" t="str">
         <f>Futures!H30</f>
-        <v>obj_00374#0000</v>
+        <v>obj_00367#0002</v>
       </c>
       <c r="F48" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E48),"LastFixing","D"),"Libor","")</f>
@@ -6725,7 +6755,7 @@
       </c>
       <c r="E49" s="117" t="str">
         <f>Futures!H31</f>
-        <v>obj_0033a#0000</v>
+        <v>obj_0034f#0002</v>
       </c>
       <c r="F49" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E49),"LastFixing","D"),"Libor","")</f>
@@ -6771,7 +6801,7 @@
       </c>
       <c r="E50" s="117" t="str">
         <f>Futures!H32</f>
-        <v>obj_00345#0000</v>
+        <v>obj_00368#0002</v>
       </c>
       <c r="F50" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E50),"LastFixing","D"),"Libor","")</f>
@@ -6817,7 +6847,7 @@
       </c>
       <c r="E51" s="117" t="str">
         <f>Futures!H33</f>
-        <v>obj_0036f#0000</v>
+        <v>obj_00370#0002</v>
       </c>
       <c r="F51" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E51),"LastFixing","D"),"Libor","")</f>
@@ -6863,7 +6893,7 @@
       </c>
       <c r="E52" s="117" t="str">
         <f>Futures!H34</f>
-        <v>obj_00353#0000</v>
+        <v>obj_00357#0002</v>
       </c>
       <c r="F52" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E52),"LastFixing","D"),"Libor","")</f>
@@ -6910,7 +6940,7 @@
       </c>
       <c r="E53" s="117" t="str">
         <f>Futures!H35</f>
-        <v>obj_00354#0000</v>
+        <v>obj_0036f#0002</v>
       </c>
       <c r="F53" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E53),"LastFixing","D"),"Libor","")</f>
@@ -6957,7 +6987,7 @@
       </c>
       <c r="E54" s="117" t="str">
         <f>Futures!H36</f>
-        <v>obj_0036c#0000</v>
+        <v>obj_00353#0002</v>
       </c>
       <c r="F54" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E54),"LastFixing","D"),"Libor","")</f>
@@ -7004,7 +7034,7 @@
       </c>
       <c r="E55" s="117" t="str">
         <f>Futures!H37</f>
-        <v>obj_00375#0000</v>
+        <v>obj_00369#0002</v>
       </c>
       <c r="F55" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E55),"LastFixing","D"),"Libor","")</f>
@@ -7051,7 +7081,7 @@
       </c>
       <c r="E56" s="117" t="str">
         <f>Futures!H38</f>
-        <v>obj_00371#0000</v>
+        <v>obj_00373#0002</v>
       </c>
       <c r="F56" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E56),"LastFixing","D"),"Libor","")</f>
@@ -7098,7 +7128,7 @@
       </c>
       <c r="E57" s="117" t="str">
         <f>Futures!H39</f>
-        <v>obj_00352#0000</v>
+        <v>obj_00351#0002</v>
       </c>
       <c r="F57" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E57),"LastFixing","D"),"Libor","")</f>
@@ -7145,7 +7175,7 @@
       </c>
       <c r="E58" s="117" t="str">
         <f>Futures!H40</f>
-        <v>obj_00343#0000</v>
+        <v>obj_00371#0002</v>
       </c>
       <c r="F58" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E58),"LastFixing","D"),"Libor","")</f>
@@ -7192,7 +7222,7 @@
       </c>
       <c r="E59" s="117" t="str">
         <f>Futures!H41</f>
-        <v>obj_00367#0000</v>
+        <v>obj_00363#0002</v>
       </c>
       <c r="F59" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E59),"LastFixing","D"),"Libor","")</f>
@@ -7239,7 +7269,7 @@
       </c>
       <c r="E60" s="117" t="str">
         <f>Futures!H42</f>
-        <v>obj_00347#0000</v>
+        <v>obj_00350#0002</v>
       </c>
       <c r="F60" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E60),"LastFixing","D"),"Libor","")</f>
@@ -7286,7 +7316,7 @@
       </c>
       <c r="E61" s="117" t="str">
         <f>Futures!H43</f>
-        <v>obj_0034f#0000</v>
+        <v>obj_00378#0002</v>
       </c>
       <c r="F61" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E61),"LastFixing","D"),"Libor","")</f>
@@ -7333,7 +7363,7 @@
       </c>
       <c r="E62" s="117" t="str">
         <f>Futures!H44</f>
-        <v>obj_0036e#0000</v>
+        <v>obj_0035d#0002</v>
       </c>
       <c r="F62" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E62),"LastFixing","D"),"Libor","")</f>
@@ -7379,7 +7409,7 @@
       </c>
       <c r="E63" s="117" t="str">
         <f>Swaps!K5</f>
-        <v>obj_00329#0008</v>
+        <v>obj_00339#0003</v>
       </c>
       <c r="F63" s="133" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E63),"LastFixing","D"),"Libor","")</f>
@@ -7387,7 +7417,7 @@
       </c>
       <c r="G63" s="134">
         <f>_xll.qlRateHelperQuoteValue($E63,Trigger)</f>
-        <v>1.4250000000000001E-3</v>
+        <v>1.4499999999999999E-3</v>
       </c>
       <c r="H63" s="134">
         <f>_xll.qlSwapRateHelperSpread($E63,Trigger)</f>
@@ -7404,11 +7434,11 @@
       </c>
       <c r="L63" s="136">
         <f>_xll.qlRateHelperEarliestDate($E63,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M63" s="137">
         <f>_xll.qlRateHelperLatestDate($E63,Trigger)</f>
-        <v>42368</v>
+        <v>42398</v>
       </c>
       <c r="O63" s="138"/>
     </row>
@@ -7425,7 +7455,7 @@
       </c>
       <c r="E64" s="117" t="str">
         <f>Swaps!K6</f>
-        <v>obj_0032e#0002</v>
+        <v>obj_0033e#0003</v>
       </c>
       <c r="F64" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E64),"LastFixing","D"),"Libor","")</f>
@@ -7450,11 +7480,11 @@
       </c>
       <c r="L64" s="119">
         <f>_xll.qlRateHelperEarliestDate($E64,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M64" s="120">
         <f>_xll.qlRateHelperLatestDate($E64,Trigger)</f>
-        <v>42459</v>
+        <v>42489</v>
       </c>
       <c r="O64" s="138"/>
     </row>
@@ -7471,7 +7501,7 @@
       </c>
       <c r="E65" s="117" t="str">
         <f>Swaps!K7</f>
-        <v>obj_00370#0002</v>
+        <v>obj_0032c#0003</v>
       </c>
       <c r="F65" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E65),"LastFixing","D"),"Libor","")</f>
@@ -7496,11 +7526,11 @@
       </c>
       <c r="L65" s="119">
         <f>_xll.qlRateHelperEarliestDate($E65,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M65" s="120">
         <f>_xll.qlRateHelperLatestDate($E65,Trigger)</f>
-        <v>42551</v>
+        <v>42580</v>
       </c>
       <c r="O65" s="138"/>
     </row>
@@ -7517,7 +7547,7 @@
       </c>
       <c r="E66" s="117" t="str">
         <f>Swaps!K8</f>
-        <v>obj_0032d#0002</v>
+        <v>obj_00338#0003</v>
       </c>
       <c r="F66" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E66),"LastFixing","D"),"Libor","")</f>
@@ -7542,11 +7572,11 @@
       </c>
       <c r="L66" s="119">
         <f>_xll.qlRateHelperEarliestDate($E66,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M66" s="120">
         <f>_xll.qlRateHelperLatestDate($E66,Trigger)</f>
-        <v>42643</v>
+        <v>42674</v>
       </c>
       <c r="O66" s="138"/>
     </row>
@@ -7563,7 +7593,7 @@
       </c>
       <c r="E67" s="117" t="str">
         <f>Swaps!K9</f>
-        <v>obj_00330#0002</v>
+        <v>obj_00346#0003</v>
       </c>
       <c r="F67" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E67),"LastFixing","D"),"Libor","")</f>
@@ -7571,7 +7601,7 @@
       </c>
       <c r="G67" s="118">
         <f>_xll.qlRateHelperQuoteValue($E67,Trigger)</f>
-        <v>1.4250000000000001E-3</v>
+        <v>1.4499999999999999E-3</v>
       </c>
       <c r="H67" s="118">
         <f>_xll.qlSwapRateHelperSpread($E67,Trigger)</f>
@@ -7588,11 +7618,11 @@
       </c>
       <c r="L67" s="119">
         <f>_xll.qlRateHelperEarliestDate($E67,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M67" s="120">
         <f>_xll.qlRateHelperLatestDate($E67,Trigger)</f>
-        <v>42734</v>
+        <v>42765</v>
       </c>
       <c r="O67" s="138"/>
     </row>
@@ -7609,7 +7639,7 @@
       </c>
       <c r="E68" s="117" t="str">
         <f>Swaps!K10</f>
-        <v>obj_00361#0002</v>
+        <v>obj_0032f#0003</v>
       </c>
       <c r="F68" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E68),"LastFixing","D"),"Libor","")</f>
@@ -7617,7 +7647,7 @@
       </c>
       <c r="G68" s="118">
         <f>_xll.qlRateHelperQuoteValue($E68,Trigger)</f>
-        <v>1.5249999999999999E-3</v>
+        <v>1.6250000000000001E-3</v>
       </c>
       <c r="H68" s="118">
         <f>_xll.qlSwapRateHelperSpread($E68,Trigger)</f>
@@ -7634,11 +7664,11 @@
       </c>
       <c r="L68" s="119">
         <f>_xll.qlRateHelperEarliestDate($E68,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M68" s="120">
         <f>_xll.qlRateHelperLatestDate($E68,Trigger)</f>
-        <v>43098</v>
+        <v>43130</v>
       </c>
       <c r="O68" s="138"/>
     </row>
@@ -7655,7 +7685,7 @@
       </c>
       <c r="E69" s="117" t="str">
         <f>Swaps!K11</f>
-        <v>obj_00358#0002</v>
+        <v>obj_00340#0003</v>
       </c>
       <c r="F69" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E69),"LastFixing","D"),"Libor","")</f>
@@ -7663,7 +7693,7 @@
       </c>
       <c r="G69" s="118">
         <f>_xll.qlRateHelperQuoteValue($E69,Trigger)</f>
-        <v>1.7750000000000001E-3</v>
+        <v>1.9500000000000001E-3</v>
       </c>
       <c r="H69" s="118">
         <f>_xll.qlSwapRateHelperSpread($E69,Trigger)</f>
@@ -7680,11 +7710,11 @@
       </c>
       <c r="L69" s="119">
         <f>_xll.qlRateHelperEarliestDate($E69,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M69" s="120">
         <f>_xll.qlRateHelperLatestDate($E69,Trigger)</f>
-        <v>43462</v>
+        <v>43495</v>
       </c>
       <c r="O69" s="138"/>
     </row>
@@ -7701,7 +7731,7 @@
       </c>
       <c r="E70" s="117" t="str">
         <f>Swaps!K12</f>
-        <v>obj_00373#0002</v>
+        <v>obj_0032e#0003</v>
       </c>
       <c r="F70" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E70),"LastFixing","D"),"Libor","")</f>
@@ -7709,7 +7739,7 @@
       </c>
       <c r="G70" s="118">
         <f>_xll.qlRateHelperQuoteValue($E70,Trigger)</f>
-        <v>2.1749999999999999E-3</v>
+        <v>2.4000000000000002E-3</v>
       </c>
       <c r="H70" s="118">
         <f>_xll.qlSwapRateHelperSpread($E70,Trigger)</f>
@@ -7726,11 +7756,11 @@
       </c>
       <c r="L70" s="119">
         <f>_xll.qlRateHelperEarliestDate($E70,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M70" s="120">
         <f>_xll.qlRateHelperLatestDate($E70,Trigger)</f>
-        <v>43829</v>
+        <v>43860</v>
       </c>
       <c r="O70" s="138"/>
     </row>
@@ -7747,7 +7777,7 @@
       </c>
       <c r="E71" s="117" t="str">
         <f>Swaps!K13</f>
-        <v>obj_00359#0002</v>
+        <v>obj_0033f#0003</v>
       </c>
       <c r="F71" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E71),"LastFixing","D"),"Libor","")</f>
@@ -7755,7 +7785,7 @@
       </c>
       <c r="G71" s="118">
         <f>_xll.qlRateHelperQuoteValue($E71,Trigger)</f>
-        <v>2.6749999999999994E-3</v>
+        <v>2.9000000000000002E-3</v>
       </c>
       <c r="H71" s="118">
         <f>_xll.qlSwapRateHelperSpread($E71,Trigger)</f>
@@ -7772,11 +7802,11 @@
       </c>
       <c r="L71" s="119">
         <f>_xll.qlRateHelperEarliestDate($E71,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M71" s="120">
         <f>_xll.qlRateHelperLatestDate($E71,Trigger)</f>
-        <v>44195</v>
+        <v>44225</v>
       </c>
       <c r="O71" s="138"/>
     </row>
@@ -7793,7 +7823,7 @@
       </c>
       <c r="E72" s="117" t="str">
         <f>Swaps!K14</f>
-        <v>obj_00363#0002</v>
+        <v>obj_00331#0003</v>
       </c>
       <c r="F72" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E72),"LastFixing","D"),"Libor","")</f>
@@ -7801,7 +7831,7 @@
       </c>
       <c r="G72" s="118">
         <f>_xll.qlRateHelperQuoteValue($E72,Trigger)</f>
-        <v>3.2500000000000003E-3</v>
+        <v>3.4250000000000001E-3</v>
       </c>
       <c r="H72" s="118">
         <f>_xll.qlSwapRateHelperSpread($E72,Trigger)</f>
@@ -7818,11 +7848,11 @@
       </c>
       <c r="L72" s="119">
         <f>_xll.qlRateHelperEarliestDate($E72,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M72" s="120">
         <f>_xll.qlRateHelperLatestDate($E72,Trigger)</f>
-        <v>44560</v>
+        <v>44592</v>
       </c>
       <c r="O72" s="138"/>
     </row>
@@ -7839,7 +7869,7 @@
       </c>
       <c r="E73" s="117" t="str">
         <f>Swaps!K15</f>
-        <v>obj_0035f#0002</v>
+        <v>obj_0034c#0003</v>
       </c>
       <c r="F73" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E73),"LastFixing","D"),"Libor","")</f>
@@ -7847,7 +7877,7 @@
       </c>
       <c r="G73" s="118">
         <f>_xll.qlRateHelperQuoteValue($E73,Trigger)</f>
-        <v>3.875E-3</v>
+        <v>3.9750000000000002E-3</v>
       </c>
       <c r="H73" s="118">
         <f>_xll.qlSwapRateHelperSpread($E73,Trigger)</f>
@@ -7864,11 +7894,11 @@
       </c>
       <c r="L73" s="119">
         <f>_xll.qlRateHelperEarliestDate($E73,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M73" s="120">
         <f>_xll.qlRateHelperLatestDate($E73,Trigger)</f>
-        <v>44925</v>
+        <v>44956</v>
       </c>
       <c r="O73" s="138"/>
     </row>
@@ -7885,7 +7915,7 @@
       </c>
       <c r="E74" s="117" t="str">
         <f>Swaps!K16</f>
-        <v>obj_0033e#0002</v>
+        <v>obj_00334#0003</v>
       </c>
       <c r="F74" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E74),"LastFixing","D"),"Libor","")</f>
@@ -7893,7 +7923,7 @@
       </c>
       <c r="G74" s="118">
         <f>_xll.qlRateHelperQuoteValue($E74,Trigger)</f>
-        <v>4.5499999999999994E-3</v>
+        <v>4.5250000000000004E-3</v>
       </c>
       <c r="H74" s="118">
         <f>_xll.qlSwapRateHelperSpread($E74,Trigger)</f>
@@ -7910,11 +7940,11 @@
       </c>
       <c r="L74" s="119">
         <f>_xll.qlRateHelperEarliestDate($E74,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M74" s="120">
         <f>_xll.qlRateHelperLatestDate($E74,Trigger)</f>
-        <v>45289</v>
+        <v>45321</v>
       </c>
       <c r="O74" s="138"/>
     </row>
@@ -7931,7 +7961,7 @@
       </c>
       <c r="E75" s="117" t="str">
         <f>Swaps!K17</f>
-        <v>obj_00372#0002</v>
+        <v>obj_00341#0003</v>
       </c>
       <c r="F75" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E75),"LastFixing","D"),"Libor","")</f>
@@ -7939,7 +7969,7 @@
       </c>
       <c r="G75" s="118">
         <f>_xll.qlRateHelperQuoteValue($E75,Trigger)</f>
-        <v>5.2249999999999996E-3</v>
+        <v>5.1000000000000004E-3</v>
       </c>
       <c r="H75" s="118">
         <f>_xll.qlSwapRateHelperSpread($E75,Trigger)</f>
@@ -7956,11 +7986,11 @@
       </c>
       <c r="L75" s="119">
         <f>_xll.qlRateHelperEarliestDate($E75,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M75" s="120">
         <f>_xll.qlRateHelperLatestDate($E75,Trigger)</f>
-        <v>45656</v>
+        <v>45687</v>
       </c>
       <c r="O75" s="138"/>
     </row>
@@ -7977,7 +8007,7 @@
       </c>
       <c r="E76" s="117" t="str">
         <f>Swaps!K18</f>
-        <v>obj_0033c#0002</v>
+        <v>obj_0032a#0003</v>
       </c>
       <c r="F76" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E76),"LastFixing","D"),"Libor","")</f>
@@ -8002,11 +8032,11 @@
       </c>
       <c r="L76" s="119">
         <f>_xll.qlRateHelperEarliestDate($E76,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M76" s="120">
         <f>_xll.qlRateHelperLatestDate($E76,Trigger)</f>
-        <v>46021</v>
+        <v>46052</v>
       </c>
       <c r="O76" s="138"/>
     </row>
@@ -8023,7 +8053,7 @@
       </c>
       <c r="E77" s="117" t="str">
         <f>Swaps!K19</f>
-        <v>obj_0034d#0002</v>
+        <v>obj_0033b#0003</v>
       </c>
       <c r="F77" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E77),"LastFixing","D"),"Libor","")</f>
@@ -8031,7 +8061,7 @@
       </c>
       <c r="G77" s="118">
         <f>_xll.qlRateHelperQuoteValue($E77,Trigger)</f>
-        <v>6.5999999999999991E-3</v>
+        <v>6.3000000000000009E-3</v>
       </c>
       <c r="H77" s="118">
         <f>_xll.qlSwapRateHelperSpread($E77,Trigger)</f>
@@ -8048,11 +8078,11 @@
       </c>
       <c r="L77" s="119">
         <f>_xll.qlRateHelperEarliestDate($E77,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M77" s="120">
         <f>_xll.qlRateHelperLatestDate($E77,Trigger)</f>
-        <v>46386</v>
+        <v>46416</v>
       </c>
       <c r="O77" s="138"/>
     </row>
@@ -8069,7 +8099,7 @@
       </c>
       <c r="E78" s="117" t="str">
         <f>Swaps!K20</f>
-        <v>obj_0036a#0002</v>
+        <v>obj_00329#0003</v>
       </c>
       <c r="F78" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E78),"LastFixing","D"),"Libor","")</f>
@@ -8094,11 +8124,11 @@
       </c>
       <c r="L78" s="119">
         <f>_xll.qlRateHelperEarliestDate($E78,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M78" s="120">
         <f>_xll.qlRateHelperLatestDate($E78,Trigger)</f>
-        <v>46751</v>
+        <v>46783</v>
       </c>
       <c r="O78" s="138"/>
     </row>
@@ -8115,7 +8145,7 @@
       </c>
       <c r="E79" s="117" t="str">
         <f>Swaps!K21</f>
-        <v>obj_0035b#0002</v>
+        <v>obj_0033a#0003</v>
       </c>
       <c r="F79" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E79),"LastFixing","D"),"Libor","")</f>
@@ -8140,11 +8170,11 @@
       </c>
       <c r="L79" s="119">
         <f>_xll.qlRateHelperEarliestDate($E79,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M79" s="120">
         <f>_xll.qlRateHelperLatestDate($E79,Trigger)</f>
-        <v>47116</v>
+        <v>47148</v>
       </c>
       <c r="O79" s="138"/>
     </row>
@@ -8161,7 +8191,7 @@
       </c>
       <c r="E80" s="117" t="str">
         <f>Swaps!K22</f>
-        <v>obj_0034b#0002</v>
+        <v>obj_0032d#0003</v>
       </c>
       <c r="F80" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E80),"LastFixing","D"),"Libor","")</f>
@@ -8169,7 +8199,7 @@
       </c>
       <c r="G80" s="118">
         <f>_xll.qlRateHelperQuoteValue($E80,Trigger)</f>
-        <v>8.8000000000000005E-3</v>
+        <v>8.2500000000000004E-3</v>
       </c>
       <c r="H80" s="118">
         <f>_xll.qlSwapRateHelperSpread($E80,Trigger)</f>
@@ -8186,11 +8216,11 @@
       </c>
       <c r="L80" s="119">
         <f>_xll.qlRateHelperEarliestDate($E80,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M80" s="120">
         <f>_xll.qlRateHelperLatestDate($E80,Trigger)</f>
-        <v>47480</v>
+        <v>47513</v>
       </c>
       <c r="O80" s="138"/>
     </row>
@@ -8207,7 +8237,7 @@
       </c>
       <c r="E81" s="117" t="str">
         <f>Swaps!K23</f>
-        <v>obj_00339#0002</v>
+        <v>obj_00347#0003</v>
       </c>
       <c r="F81" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E81),"LastFixing","D"),"Libor","")</f>
@@ -8232,11 +8262,11 @@
       </c>
       <c r="L81" s="119">
         <f>_xll.qlRateHelperEarliestDate($E81,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M81" s="120">
         <f>_xll.qlRateHelperLatestDate($E81,Trigger)</f>
-        <v>47847</v>
+        <v>47878</v>
       </c>
       <c r="O81" s="138"/>
     </row>
@@ -8253,7 +8283,7 @@
       </c>
       <c r="E82" s="117" t="str">
         <f>Swaps!K24</f>
-        <v>obj_0033b#0002</v>
+        <v>obj_00330#0003</v>
       </c>
       <c r="F82" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E82),"LastFixing","D"),"Libor","")</f>
@@ -8278,11 +8308,11 @@
       </c>
       <c r="L82" s="119">
         <f>_xll.qlRateHelperEarliestDate($E82,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M82" s="120">
         <f>_xll.qlRateHelperLatestDate($E82,Trigger)</f>
-        <v>48212</v>
+        <v>48243</v>
       </c>
       <c r="O82" s="138"/>
     </row>
@@ -8299,7 +8329,7 @@
       </c>
       <c r="E83" s="117" t="str">
         <f>Swaps!K25</f>
-        <v>obj_00335#0002</v>
+        <v>obj_0033c#0003</v>
       </c>
       <c r="F83" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E83),"LastFixing","D"),"Libor","")</f>
@@ -8324,11 +8354,11 @@
       </c>
       <c r="L83" s="119">
         <f>_xll.qlRateHelperEarliestDate($E83,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M83" s="120">
         <f>_xll.qlRateHelperLatestDate($E83,Trigger)</f>
-        <v>48578</v>
+        <v>48610</v>
       </c>
       <c r="O83" s="138"/>
     </row>
@@ -8345,7 +8375,7 @@
       </c>
       <c r="E84" s="117" t="str">
         <f>Swaps!K26</f>
-        <v>obj_0035a#0002</v>
+        <v>obj_0034a#0003</v>
       </c>
       <c r="F84" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E84),"LastFixing","D"),"Libor","")</f>
@@ -8370,11 +8400,11 @@
       </c>
       <c r="L84" s="119">
         <f>_xll.qlRateHelperEarliestDate($E84,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M84" s="120">
         <f>_xll.qlRateHelperLatestDate($E84,Trigger)</f>
-        <v>48943</v>
+        <v>48974</v>
       </c>
       <c r="O84" s="138"/>
     </row>
@@ -8391,7 +8421,7 @@
       </c>
       <c r="E85" s="117" t="str">
         <f>Swaps!K27</f>
-        <v>obj_00356#0002</v>
+        <v>obj_00336#0003</v>
       </c>
       <c r="F85" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E85),"LastFixing","D"),"Libor","")</f>
@@ -8399,7 +8429,7 @@
       </c>
       <c r="G85" s="118">
         <f>_xll.qlRateHelperQuoteValue($E85,Trigger)</f>
-        <v>1.1575E-2</v>
+        <v>1.0874999999999999E-2</v>
       </c>
       <c r="H85" s="118">
         <f>_xll.qlSwapRateHelperSpread($E85,Trigger)</f>
@@ -8416,11 +8446,11 @@
       </c>
       <c r="L85" s="119">
         <f>_xll.qlRateHelperEarliestDate($E85,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M85" s="120">
         <f>_xll.qlRateHelperLatestDate($E85,Trigger)</f>
-        <v>49307</v>
+        <v>49339</v>
       </c>
       <c r="O85" s="138"/>
     </row>
@@ -8437,7 +8467,7 @@
       </c>
       <c r="E86" s="117" t="str">
         <f>Swaps!K28</f>
-        <v>obj_0036b#0002</v>
+        <v>obj_00349#0003</v>
       </c>
       <c r="F86" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E86),"LastFixing","D"),"Libor","")</f>
@@ -8462,11 +8492,11 @@
       </c>
       <c r="L86" s="119">
         <f>_xll.qlRateHelperEarliestDate($E86,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M86" s="120">
         <f>_xll.qlRateHelperLatestDate($E86,Trigger)</f>
-        <v>49671</v>
+        <v>49704</v>
       </c>
       <c r="O86" s="138"/>
     </row>
@@ -8483,7 +8513,7 @@
       </c>
       <c r="E87" s="117" t="str">
         <f>Swaps!K29</f>
-        <v>obj_00350#0002</v>
+        <v>obj_00335#0003</v>
       </c>
       <c r="F87" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E87),"LastFixing","D"),"Libor","")</f>
@@ -8508,11 +8538,11 @@
       </c>
       <c r="L87" s="119">
         <f>_xll.qlRateHelperEarliestDate($E87,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M87" s="120">
         <f>_xll.qlRateHelperLatestDate($E87,Trigger)</f>
-        <v>50039</v>
+        <v>50070</v>
       </c>
       <c r="O87" s="138"/>
     </row>
@@ -8529,7 +8559,7 @@
       </c>
       <c r="E88" s="117" t="str">
         <f>Swaps!K30</f>
-        <v>obj_0032b#0002</v>
+        <v>obj_00328#0003</v>
       </c>
       <c r="F88" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E88),"LastFixing","D"),"Libor","")</f>
@@ -8554,11 +8584,11 @@
       </c>
       <c r="L88" s="119">
         <f>_xll.qlRateHelperEarliestDate($E88,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M88" s="120">
         <f>_xll.qlRateHelperLatestDate($E88,Trigger)</f>
-        <v>50404</v>
+        <v>50434</v>
       </c>
       <c r="O88" s="138"/>
     </row>
@@ -8575,7 +8605,7 @@
       </c>
       <c r="E89" s="117" t="str">
         <f>Swaps!K31</f>
-        <v>obj_00334#0002</v>
+        <v>obj_00342#0003</v>
       </c>
       <c r="F89" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E89),"LastFixing","D"),"Libor","")</f>
@@ -8600,11 +8630,11 @@
       </c>
       <c r="L89" s="119">
         <f>_xll.qlRateHelperEarliestDate($E89,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M89" s="120">
         <f>_xll.qlRateHelperLatestDate($E89,Trigger)</f>
-        <v>50769</v>
+        <v>50801</v>
       </c>
       <c r="O89" s="138"/>
     </row>
@@ -8621,7 +8651,7 @@
       </c>
       <c r="E90" s="117" t="str">
         <f>Swaps!K32</f>
-        <v>obj_00357#0002</v>
+        <v>obj_0032b#0003</v>
       </c>
       <c r="F90" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E90),"LastFixing","D"),"Libor","")</f>
@@ -8629,7 +8659,7 @@
       </c>
       <c r="G90" s="118">
         <f>_xll.qlRateHelperQuoteValue($E90,Trigger)</f>
-        <v>1.3050000000000001E-2</v>
+        <v>1.2275000000000001E-2</v>
       </c>
       <c r="H90" s="118">
         <f>_xll.qlSwapRateHelperSpread($E90,Trigger)</f>
@@ -8646,11 +8676,11 @@
       </c>
       <c r="L90" s="119">
         <f>_xll.qlRateHelperEarliestDate($E90,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M90" s="120">
         <f>_xll.qlRateHelperLatestDate($E90,Trigger)</f>
-        <v>51134</v>
+        <v>51165</v>
       </c>
     </row>
     <row r="91" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8666,7 +8696,7 @@
       </c>
       <c r="E91" s="117" t="str">
         <f>Swaps!K33</f>
-        <v>obj_00364#0002</v>
+        <v>obj_00337#0003</v>
       </c>
       <c r="F91" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E91),"LastFixing","D"),"Libor","")</f>
@@ -8691,11 +8721,11 @@
       </c>
       <c r="L91" s="119">
         <f>_xll.qlRateHelperEarliestDate($E91,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M91" s="120">
         <f>_xll.qlRateHelperLatestDate($E91,Trigger)</f>
-        <v>51498</v>
+        <v>51531</v>
       </c>
     </row>
     <row r="92" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8711,7 +8741,7 @@
       </c>
       <c r="E92" s="117" t="str">
         <f>Swaps!K34</f>
-        <v>obj_00369#0002</v>
+        <v>obj_00345#0003</v>
       </c>
       <c r="F92" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E92),"LastFixing","D"),"Libor","")</f>
@@ -8736,11 +8766,11 @@
       </c>
       <c r="L92" s="119">
         <f>_xll.qlRateHelperEarliestDate($E92,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M92" s="120">
         <f>_xll.qlRateHelperLatestDate($E92,Trigger)</f>
-        <v>51865</v>
+        <v>51896</v>
       </c>
     </row>
     <row r="93" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8756,7 +8786,7 @@
       </c>
       <c r="E93" s="117" t="str">
         <f>Swaps!K35</f>
-        <v>obj_00338#0002</v>
+        <v>obj_00332#0003</v>
       </c>
       <c r="F93" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E93),"LastFixing","D"),"Libor","")</f>
@@ -8781,11 +8811,11 @@
       </c>
       <c r="L93" s="119">
         <f>_xll.qlRateHelperEarliestDate($E93,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M93" s="120">
         <f>_xll.qlRateHelperLatestDate($E93,Trigger)</f>
-        <v>52230</v>
+        <v>52261</v>
       </c>
     </row>
     <row r="94" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8801,7 +8831,7 @@
       </c>
       <c r="E94" s="117" t="str">
         <f>Swaps!K36</f>
-        <v>obj_0032c#0002</v>
+        <v>obj_00344#0003</v>
       </c>
       <c r="F94" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E94),"LastFixing","D"),"Libor","")</f>
@@ -8826,11 +8856,11 @@
       </c>
       <c r="L94" s="119">
         <f>_xll.qlRateHelperEarliestDate($E94,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M94" s="120">
         <f>_xll.qlRateHelperLatestDate($E94,Trigger)</f>
-        <v>52595</v>
+        <v>52625</v>
       </c>
     </row>
     <row r="95" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8846,7 +8876,7 @@
       </c>
       <c r="E95" s="117" t="str">
         <f>Swaps!K37</f>
-        <v>obj_00341#0002</v>
+        <v>obj_00343#0003</v>
       </c>
       <c r="F95" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E95),"LastFixing","D"),"Libor","")</f>
@@ -8854,7 +8884,7 @@
       </c>
       <c r="G95" s="118">
         <f>_xll.qlRateHelperQuoteValue($E95,Trigger)</f>
-        <v>1.3824999999999999E-2</v>
+        <v>1.2999999999999998E-2</v>
       </c>
       <c r="H95" s="118">
         <f>_xll.qlSwapRateHelperSpread($E95,Trigger)</f>
@@ -8871,11 +8901,11 @@
       </c>
       <c r="L95" s="119">
         <f>_xll.qlRateHelperEarliestDate($E95,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M95" s="120">
         <f>_xll.qlRateHelperLatestDate($E95,Trigger)</f>
-        <v>52961</v>
+        <v>52992</v>
       </c>
     </row>
     <row r="96" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8891,7 +8921,7 @@
       </c>
       <c r="E96" s="117" t="str">
         <f>Swaps!K38</f>
-        <v>obj_0033d#0002</v>
+        <v>obj_00348#0003</v>
       </c>
       <c r="F96" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E96),"LastFixing","D"),"Libor","")</f>
@@ -8916,11 +8946,11 @@
       </c>
       <c r="L96" s="119">
         <f>_xll.qlRateHelperEarliestDate($E96,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M96" s="120">
         <f>_xll.qlRateHelperLatestDate($E96,Trigger)</f>
-        <v>54787</v>
+        <v>54819</v>
       </c>
     </row>
     <row r="97" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8936,7 +8966,7 @@
       </c>
       <c r="E97" s="117" t="str">
         <f>Swaps!K39</f>
-        <v>obj_00337#0002</v>
+        <v>obj_0033d#0003</v>
       </c>
       <c r="F97" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E97),"LastFixing","D"),"Libor","")</f>
@@ -8961,11 +8991,11 @@
       </c>
       <c r="L97" s="119">
         <f>_xll.qlRateHelperEarliestDate($E97,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M97" s="120">
         <f>_xll.qlRateHelperLatestDate($E97,Trigger)</f>
-        <v>56613</v>
+        <v>56643</v>
       </c>
     </row>
     <row r="98" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8981,7 +9011,7 @@
       </c>
       <c r="E98" s="117" t="str">
         <f>Swaps!K40</f>
-        <v>obj_00333#0002</v>
+        <v>obj_0034b#0003</v>
       </c>
       <c r="F98" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E98),"LastFixing","D"),"Libor","")</f>
@@ -9006,11 +9036,11 @@
       </c>
       <c r="L98" s="119">
         <f>_xll.qlRateHelperEarliestDate($E98,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M98" s="120">
         <f>_xll.qlRateHelperLatestDate($E98,Trigger)</f>
-        <v>60266</v>
+        <v>60297</v>
       </c>
     </row>
     <row r="99" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9026,7 +9056,7 @@
       </c>
       <c r="E99" s="117" t="str">
         <f>Swaps!K41</f>
-        <v>obj_00366#0002</v>
+        <v>obj_00333#0003</v>
       </c>
       <c r="F99" s="117" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(E99),"LastFixing","D"),"Libor","")</f>
@@ -9051,11 +9081,11 @@
       </c>
       <c r="L99" s="125">
         <f>_xll.qlRateHelperEarliestDate($E99,Trigger)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="M99" s="126">
         <f>_xll.qlRateHelperLatestDate($E99,Trigger)</f>
-        <v>63916</v>
+        <v>63949</v>
       </c>
     </row>
     <row r="100" spans="2:13" x14ac:dyDescent="0.25">
@@ -9120,7 +9150,7 @@
       </c>
       <c r="J1" s="75">
         <f t="array" ref="J1:J126">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
-        <v>5.3593891239512345E-4</v>
+        <v>4.1275253303319951E-4</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -9132,7 +9162,7 @@
       </c>
       <c r="D2" s="76" t="str">
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
-        <v>obj_00320</v>
+        <v>obj_00319</v>
       </c>
       <c r="E2" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D2),"LastFixing","D"),"Libor","")</f>
@@ -9140,7 +9170,7 @@
       </c>
       <c r="F2" s="77">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>5.2859999999999995E-4</v>
+        <v>4.0709999999999997E-4</v>
       </c>
       <c r="G2" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -9148,14 +9178,14 @@
       </c>
       <c r="H2" s="86">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I2" s="87">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>42010</v>
+        <v>42041</v>
       </c>
       <c r="J2" s="75">
-        <v>5.3593891239512345E-4</v>
+        <v>4.1275253303319951E-4</v>
       </c>
       <c r="K2" s="78"/>
     </row>
@@ -9167,7 +9197,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="76" t="str">
-        <v>obj_00326</v>
+        <v>obj_00327</v>
       </c>
       <c r="E3" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D3),"LastFixing","D"),"Libor","")</f>
@@ -9175,7 +9205,7 @@
       </c>
       <c r="F3" s="77">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>7.2859999999999993E-4</v>
+        <v>7.1429999999999996E-4</v>
       </c>
       <c r="G3" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -9183,14 +9213,14 @@
       </c>
       <c r="H3" s="86">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I3" s="87">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>42034</v>
+        <v>42062</v>
       </c>
       <c r="J3" s="75">
-        <v>7.0581669981910518E-4</v>
+        <v>7.0343750420393306E-4</v>
       </c>
       <c r="K3" s="78"/>
     </row>
@@ -9202,7 +9232,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="76" t="str">
-        <v>obj_0031c</v>
+        <v>obj_00320</v>
       </c>
       <c r="E4" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D4),"LastFixing","D"),"Libor","")</f>
@@ -9210,7 +9240,7 @@
       </c>
       <c r="F4" s="77">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>9.5E-4</v>
+        <v>9.0709999999999999E-4</v>
       </c>
       <c r="G4" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -9218,14 +9248,14 @@
       </c>
       <c r="H4" s="86">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I4" s="87">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>42062</v>
+        <v>42094</v>
       </c>
       <c r="J4" s="75">
-        <v>9.2368741856078875E-4</v>
+        <v>9.0327823967882961E-4</v>
       </c>
       <c r="K4" s="78"/>
     </row>
@@ -9237,7 +9267,7 @@
         <v>52</v>
       </c>
       <c r="D5" s="76" t="str">
-        <v>obj_00322</v>
+        <v>obj_0031d</v>
       </c>
       <c r="E5" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D5),"LastFixing","D"),"Libor","")</f>
@@ -9245,7 +9275,7 @@
       </c>
       <c r="F5" s="77">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>1.1142999999999999E-3</v>
+        <v>1.0214E-3</v>
       </c>
       <c r="G5" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -9253,14 +9283,14 @@
       </c>
       <c r="H5" s="86">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I5" s="87">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>42093</v>
+        <v>42124</v>
       </c>
       <c r="J5" s="75">
-        <v>1.0925140455052213E-3</v>
+        <v>1.0219169285902441E-3</v>
       </c>
       <c r="K5" s="78"/>
     </row>
@@ -9273,7 +9303,7 @@
         <v/>
       </c>
       <c r="D6" s="76" t="str">
-        <v>obj_00325</v>
+        <v>obj_00324</v>
       </c>
       <c r="E6" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D6),"LastFixing","D"),"Libor","")</f>
@@ -9281,7 +9311,7 @@
       </c>
       <c r="F6" s="77">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>1.4513999999999998E-3</v>
+        <v>1.4357E-3</v>
       </c>
       <c r="G6" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
@@ -9289,20 +9319,20 @@
       </c>
       <c r="H6" s="86">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I6" s="87">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>42185</v>
+        <v>42216</v>
       </c>
       <c r="J6" s="75">
-        <v>1.4411757372655499E-3</v>
+        <v>1.4437822653410373E-3</v>
       </c>
       <c r="K6" s="78"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D7" s="76" t="str">
-        <v>obj_00329</v>
+        <v>obj_00339</v>
       </c>
       <c r="E7" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D7),"LastFixing","D"),"Libor","")</f>
@@ -9310,7 +9340,7 @@
       </c>
       <c r="F7" s="77">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>1.4250000000000001E-3</v>
+        <v>1.4499999999999999E-3</v>
       </c>
       <c r="G7" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -9318,20 +9348,20 @@
       </c>
       <c r="H7" s="86">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I7" s="87">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>42368</v>
+        <v>42398</v>
       </c>
       <c r="J7" s="75">
-        <v>1.4101062237897141E-3</v>
+        <v>1.441545667596451E-3</v>
       </c>
       <c r="K7" s="78"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D8" s="76" t="str">
-        <v>obj_00370</v>
+        <v>obj_0032c</v>
       </c>
       <c r="E8" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D8),"LastFixing","D"),"Libor","")</f>
@@ -9347,20 +9377,20 @@
       </c>
       <c r="H8" s="86">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I8" s="87">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>42551</v>
+        <v>42580</v>
       </c>
       <c r="J8" s="75">
-        <v>1.4148579381860508E-3</v>
+        <v>1.4192709018787935E-3</v>
       </c>
       <c r="K8" s="78"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D9" s="76" t="str">
-        <v>obj_00361</v>
+        <v>obj_0032f</v>
       </c>
       <c r="E9" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D9),"LastFixing","D"),"Libor","")</f>
@@ -9368,7 +9398,7 @@
       </c>
       <c r="F9" s="77">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>1.5249999999999999E-3</v>
+        <v>1.6250000000000001E-3</v>
       </c>
       <c r="G9" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -9376,20 +9406,20 @@
       </c>
       <c r="H9" s="86">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I9" s="87">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>43098</v>
+        <v>43130</v>
       </c>
       <c r="J9" s="75">
-        <v>1.5191576859674095E-3</v>
+        <v>1.6216466863902467E-3</v>
       </c>
       <c r="K9" s="78"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D10" s="76" t="str">
-        <v>obj_00358</v>
+        <v>obj_00340</v>
       </c>
       <c r="E10" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D10),"LastFixing","D"),"Libor","")</f>
@@ -9397,7 +9427,7 @@
       </c>
       <c r="F10" s="77">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>1.7750000000000001E-3</v>
+        <v>1.9500000000000001E-3</v>
       </c>
       <c r="G10" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -9405,20 +9435,20 @@
       </c>
       <c r="H10" s="86">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I10" s="87">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>43462</v>
+        <v>43495</v>
       </c>
       <c r="J10" s="75">
-        <v>1.7699294984106981E-3</v>
+        <v>1.9475960365556522E-3</v>
       </c>
       <c r="K10" s="78"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D11" s="76" t="str">
-        <v>obj_00373</v>
+        <v>obj_0032e</v>
       </c>
       <c r="E11" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D11),"LastFixing","D"),"Libor","")</f>
@@ -9426,7 +9456,7 @@
       </c>
       <c r="F11" s="77">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>2.1749999999999999E-3</v>
+        <v>2.4000000000000002E-3</v>
       </c>
       <c r="G11" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -9434,20 +9464,20 @@
       </c>
       <c r="H11" s="86">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I11" s="87">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>43829</v>
+        <v>43860</v>
       </c>
       <c r="J11" s="75">
-        <v>2.1709841407449876E-3</v>
+        <v>2.3993233482298743E-3</v>
       </c>
       <c r="K11" s="78"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D12" s="76" t="str">
-        <v>obj_00359</v>
+        <v>obj_0033f</v>
       </c>
       <c r="E12" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D12),"LastFixing","D"),"Libor","")</f>
@@ -9455,7 +9485,7 @@
       </c>
       <c r="F12" s="77">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>2.6749999999999994E-3</v>
+        <v>2.9000000000000002E-3</v>
       </c>
       <c r="G12" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -9463,20 +9493,20 @@
       </c>
       <c r="H12" s="86">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I12" s="87">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>44195</v>
+        <v>44225</v>
       </c>
       <c r="J12" s="75">
-        <v>2.6733549286184384E-3</v>
+        <v>2.9023458534390843E-3</v>
       </c>
       <c r="K12" s="78"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D13" s="76" t="str">
-        <v>obj_00363</v>
+        <v>obj_00331</v>
       </c>
       <c r="E13" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D13),"LastFixing","D"),"Libor","")</f>
@@ -9484,7 +9514,7 @@
       </c>
       <c r="F13" s="77">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>3.2500000000000003E-3</v>
+        <v>3.4250000000000001E-3</v>
       </c>
       <c r="G13" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -9492,20 +9522,20 @@
       </c>
       <c r="H13" s="86">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I13" s="87">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>44560</v>
+        <v>44592</v>
       </c>
       <c r="J13" s="75">
-        <v>3.2529296428579092E-3</v>
+        <v>3.4320470500170445E-3</v>
       </c>
       <c r="K13" s="78"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D14" s="76" t="str">
-        <v>obj_0035f</v>
+        <v>obj_0034c</v>
       </c>
       <c r="E14" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D14),"LastFixing","D"),"Libor","")</f>
@@ -9513,7 +9543,7 @@
       </c>
       <c r="F14" s="77">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>3.875E-3</v>
+        <v>3.9750000000000002E-3</v>
       </c>
       <c r="G14" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -9521,20 +9551,20 @@
       </c>
       <c r="H14" s="86">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I14" s="87">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>44925</v>
+        <v>44956</v>
       </c>
       <c r="J14" s="75">
-        <v>3.8854849137784802E-3</v>
+        <v>3.9890017103214005E-3</v>
       </c>
       <c r="K14" s="78"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D15" s="76" t="str">
-        <v>obj_0033e</v>
+        <v>obj_00334</v>
       </c>
       <c r="E15" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D15),"LastFixing","D"),"Libor","")</f>
@@ -9542,7 +9572,7 @@
       </c>
       <c r="F15" s="77">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>4.5499999999999994E-3</v>
+        <v>4.5250000000000004E-3</v>
       </c>
       <c r="G15" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
@@ -9550,20 +9580,20 @@
       </c>
       <c r="H15" s="86">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I15" s="87">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>45289</v>
+        <v>45321</v>
       </c>
       <c r="J15" s="75">
-        <v>4.572114635070978E-3</v>
+        <v>4.5482512473312585E-3</v>
       </c>
       <c r="K15" s="78"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D16" s="76" t="str">
-        <v>obj_00372</v>
+        <v>obj_00341</v>
       </c>
       <c r="E16" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D16),"LastFixing","D"),"Libor","")</f>
@@ -9571,7 +9601,7 @@
       </c>
       <c r="F16" s="77">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>5.2249999999999996E-3</v>
+        <v>5.1000000000000004E-3</v>
       </c>
       <c r="G16" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
@@ -9579,19 +9609,19 @@
       </c>
       <c r="H16" s="86">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I16" s="87">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>45656</v>
+        <v>45687</v>
       </c>
       <c r="J16" s="75">
-        <v>5.2626010378304935E-3</v>
+        <v>5.1358687247593186E-3</v>
       </c>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D17" s="76" t="str">
-        <v>obj_0034d</v>
+        <v>obj_0033b</v>
       </c>
       <c r="E17" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D17),"LastFixing","D"),"Libor","")</f>
@@ -9599,7 +9629,7 @@
       </c>
       <c r="F17" s="77">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>6.5999999999999991E-3</v>
+        <v>6.3000000000000009E-3</v>
       </c>
       <c r="G17" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
@@ -9607,19 +9637,19 @@
       </c>
       <c r="H17" s="86">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I17" s="87">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>46386</v>
+        <v>46416</v>
       </c>
       <c r="J17" s="75">
-        <v>6.6835331275429486E-3</v>
+        <v>6.3734563905402022E-3</v>
       </c>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D18" s="76" t="str">
-        <v>obj_0034b</v>
+        <v>obj_0032d</v>
       </c>
       <c r="E18" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D18),"LastFixing","D"),"Libor","")</f>
@@ -9627,7 +9657,7 @@
       </c>
       <c r="F18" s="77">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>8.8000000000000005E-3</v>
+        <v>8.2500000000000004E-3</v>
       </c>
       <c r="G18" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
@@ -9635,19 +9665,19 @@
       </c>
       <c r="H18" s="86">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I18" s="87">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>47480</v>
+        <v>47513</v>
       </c>
       <c r="J18" s="75">
-        <v>9.0079998237183809E-3</v>
+        <v>8.424998637115131E-3</v>
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D19" s="76" t="str">
-        <v>obj_00356</v>
+        <v>obj_00336</v>
       </c>
       <c r="E19" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D19),"LastFixing","D"),"Libor","")</f>
@@ -9655,7 +9685,7 @@
       </c>
       <c r="F19" s="77">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>1.1575E-2</v>
+        <v>1.0874999999999999E-2</v>
       </c>
       <c r="G19" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
@@ -9663,19 +9693,19 @@
       </c>
       <c r="H19" s="86">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I19" s="87">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>49307</v>
+        <v>49339</v>
       </c>
       <c r="J19" s="75">
-        <v>1.2045876520181775E-2</v>
+        <v>1.1281939014637988E-2</v>
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D20" s="76" t="str">
-        <v>obj_00357</v>
+        <v>obj_0032b</v>
       </c>
       <c r="E20" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D20),"LastFixing","D"),"Libor","")</f>
@@ -9683,7 +9713,7 @@
       </c>
       <c r="F20" s="77">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>1.3050000000000001E-2</v>
+        <v>1.2275000000000001E-2</v>
       </c>
       <c r="G20" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
@@ -9691,19 +9721,19 @@
       </c>
       <c r="H20" s="86">
         <f>_xll.qlRateHelperEarliestDate($D20)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I20" s="87">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>51134</v>
+        <v>51165</v>
       </c>
       <c r="J20" s="75">
-        <v>1.3697570922766415E-2</v>
+        <v>1.2838816402852856E-2</v>
       </c>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D21" s="76" t="str">
-        <v>obj_00341</v>
+        <v>obj_00343</v>
       </c>
       <c r="E21" s="76" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(_xll.qlRateHelperQuoteName(D21),"LastFixing","D"),"Libor","")</f>
@@ -9711,7 +9741,7 @@
       </c>
       <c r="F21" s="77">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>1.3824999999999999E-2</v>
+        <v>1.2999999999999998E-2</v>
       </c>
       <c r="G21" s="77">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
@@ -9719,14 +9749,14 @@
       </c>
       <c r="H21" s="86">
         <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>42003</v>
+        <v>42034</v>
       </c>
       <c r="I21" s="87">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>52961</v>
+        <v>52992</v>
       </c>
       <c r="J21" s="75">
-        <v>1.4556954057314556E-2</v>
+        <v>1.3636110672599748E-2</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.2">
@@ -12757,7 +12787,7 @@
       </c>
       <c r="E3" s="51" t="str">
         <f>_xll.qlDepositRateHelper(,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0032a#0000</v>
+        <v>obj_0034e#0002</v>
       </c>
       <c r="F3" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(E3)</f>
@@ -12772,7 +12802,7 @@
       </c>
       <c r="C4" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B4,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0031f#0000</v>
+        <v>obj_00316#0002</v>
       </c>
       <c r="D4" s="52" t="str">
         <f t="shared" ref="D4:D19" si="0">PROPER(Currency)&amp;FamilyName&amp;$B4&amp;"LastFixing"&amp;QuoteSuffix</f>
@@ -12780,7 +12810,7 @@
       </c>
       <c r="E4" s="51" t="str">
         <f>_xll.qlDepositRateHelper(,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00328#0000</v>
+        <v>obj_0034d#0002</v>
       </c>
       <c r="F4" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(E4)</f>
@@ -12795,7 +12825,7 @@
       </c>
       <c r="C5" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B5,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0030a#0000</v>
+        <v>obj_00310#0002</v>
       </c>
       <c r="D5" s="52" t="str">
         <f t="shared" si="0"/>
@@ -12803,7 +12833,7 @@
       </c>
       <c r="E5" s="51" t="str">
         <f>_xll.qlDepositRateHelper(,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00320#0000</v>
+        <v>obj_00319#0002</v>
       </c>
       <c r="F5" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(E5)</f>
@@ -12818,7 +12848,7 @@
       </c>
       <c r="C6" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B6,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0030d#0000</v>
+        <v>obj_00314#0002</v>
       </c>
       <c r="D6" s="52" t="str">
         <f t="shared" si="0"/>
@@ -12838,7 +12868,7 @@
       </c>
       <c r="C7" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B7,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0030b#0000</v>
+        <v>obj_00312#0002</v>
       </c>
       <c r="D7" s="52" t="str">
         <f t="shared" si="0"/>
@@ -12858,7 +12888,7 @@
       </c>
       <c r="C8" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B8,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00311#0000</v>
+        <v>obj_0030f#0002</v>
       </c>
       <c r="D8" s="52" t="str">
         <f t="shared" si="0"/>
@@ -12866,7 +12896,7 @@
       </c>
       <c r="E8" s="51" t="str">
         <f>_xll.qlDepositRateHelper(,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00326#0000</v>
+        <v>obj_00327#0002</v>
       </c>
       <c r="F8" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -12881,7 +12911,7 @@
       </c>
       <c r="C9" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B9,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00306#0000</v>
+        <v>obj_00308#0002</v>
       </c>
       <c r="D9" s="52" t="str">
         <f t="shared" si="0"/>
@@ -12889,7 +12919,7 @@
       </c>
       <c r="E9" s="51" t="str">
         <f>_xll.qlDepositRateHelper(,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0031c#0000</v>
+        <v>obj_00320#0002</v>
       </c>
       <c r="F9" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -12904,7 +12934,7 @@
       </c>
       <c r="C10" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B10,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00308#0000</v>
+        <v>obj_0030c#0002</v>
       </c>
       <c r="D10" s="52" t="str">
         <f t="shared" si="0"/>
@@ -12912,7 +12942,7 @@
       </c>
       <c r="E10" s="51" t="str">
         <f>_xll.qlDepositRateHelper(,D10,C10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00322#0000</v>
+        <v>obj_0031d#0002</v>
       </c>
       <c r="F10" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -12927,7 +12957,7 @@
       </c>
       <c r="C11" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B11,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00310#0000</v>
+        <v>obj_0030d#0002</v>
       </c>
       <c r="D11" s="52" t="str">
         <f t="shared" si="0"/>
@@ -12947,7 +12977,7 @@
       </c>
       <c r="C12" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B12,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0030f#0000</v>
+        <v>obj_0030b#0002</v>
       </c>
       <c r="D12" s="52" t="str">
         <f t="shared" si="0"/>
@@ -12967,7 +12997,7 @@
       </c>
       <c r="C13" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B13,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0030c#0000</v>
+        <v>obj_00306#0002</v>
       </c>
       <c r="D13" s="52" t="str">
         <f t="shared" si="0"/>
@@ -12975,7 +13005,7 @@
       </c>
       <c r="E13" s="51" t="str">
         <f>_xll.qlDepositRateHelper(,D13,C13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00325#0000</v>
+        <v>obj_00324#0002</v>
       </c>
       <c r="F13" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(E13)</f>
@@ -12990,7 +13020,7 @@
       </c>
       <c r="C14" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B14,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00312#0000</v>
+        <v>obj_00311#0002</v>
       </c>
       <c r="D14" s="52" t="str">
         <f t="shared" si="0"/>
@@ -13010,7 +13040,7 @@
       </c>
       <c r="C15" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B15,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00307#0000</v>
+        <v>obj_0030a#0002</v>
       </c>
       <c r="D15" s="52" t="str">
         <f t="shared" si="0"/>
@@ -13030,7 +13060,7 @@
       </c>
       <c r="C16" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B16,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00314#0000</v>
+        <v>obj_00307#0002</v>
       </c>
       <c r="D16" s="52" t="str">
         <f t="shared" si="0"/>
@@ -13050,7 +13080,7 @@
       </c>
       <c r="C17" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B17,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00309#0000</v>
+        <v>obj_0030e#0002</v>
       </c>
       <c r="D17" s="52" t="str">
         <f t="shared" si="0"/>
@@ -13070,7 +13100,7 @@
       </c>
       <c r="C18" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B18,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_0030e#0000</v>
+        <v>obj_00309#0002</v>
       </c>
       <c r="D18" s="52" t="str">
         <f t="shared" si="0"/>
@@ -13090,7 +13120,7 @@
       </c>
       <c r="C19" s="53" t="str">
         <f>_xll.qlLibor(,Currency,B19,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_00313#0000</v>
+        <v>obj_00313#0002</v>
       </c>
       <c r="D19" s="52" t="str">
         <f t="shared" si="0"/>
@@ -13098,7 +13128,7 @@
       </c>
       <c r="E19" s="51" t="str">
         <f>_xll.qlDepositRateHelper(,D19,C19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00317#0000</v>
+        <v>obj_00315#0002</v>
       </c>
       <c r="F19" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(E19)</f>
@@ -13208,7 +13238,7 @@
       </c>
       <c r="G3" s="187" t="str">
         <f>_xll.qlFraRateHelper(,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0031d#0000</v>
+        <v>obj_00323#0002</v>
       </c>
       <c r="H3" s="188" t="str">
         <f>_xll.ohRangeRetrieveError(G3)</f>
@@ -13239,7 +13269,7 @@
       </c>
       <c r="G4" s="187" t="str">
         <f>_xll.qlFraRateHelper(,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00321#0000</v>
+        <v>obj_0031b#0002</v>
       </c>
       <c r="H4" s="188" t="str">
         <f>_xll.ohRangeRetrieveError(G4)</f>
@@ -13270,7 +13300,7 @@
       </c>
       <c r="G5" s="187" t="str">
         <f>_xll.qlFraRateHelper(,F5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00318#0000</v>
+        <v>obj_00318#0002</v>
       </c>
       <c r="H5" s="188" t="str">
         <f>_xll.ohRangeRetrieveError(G5)</f>
@@ -13301,7 +13331,7 @@
       </c>
       <c r="G6" s="187" t="str">
         <f>_xll.qlFraRateHelper(,F6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0031e#0000</v>
+        <v>obj_00326#0002</v>
       </c>
       <c r="H6" s="188" t="str">
         <f>_xll.ohRangeRetrieveError(G6)</f>
@@ -13332,7 +13362,7 @@
       </c>
       <c r="G7" s="187" t="str">
         <f>_xll.qlFraRateHelper(,F7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00316#0000</v>
+        <v>obj_00325#0002</v>
       </c>
       <c r="H7" s="188" t="str">
         <f>_xll.ohRangeRetrieveError(G7)</f>
@@ -13363,7 +13393,7 @@
       </c>
       <c r="G8" s="187" t="str">
         <f>_xll.qlFraRateHelper(,F8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00324#0000</v>
+        <v>obj_00321#0002</v>
       </c>
       <c r="H8" s="188" t="str">
         <f>_xll.ohRangeRetrieveError(G8)</f>
@@ -13394,7 +13424,7 @@
       </c>
       <c r="G9" s="187" t="str">
         <f>_xll.qlFraRateHelper(,F9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0031b#0000</v>
+        <v>obj_0031e#0002</v>
       </c>
       <c r="H9" s="188" t="str">
         <f>_xll.ohRangeRetrieveError(G9)</f>
@@ -13425,7 +13455,7 @@
       </c>
       <c r="G10" s="187" t="str">
         <f>_xll.qlFraRateHelper(,F10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00327#0000</v>
+        <v>obj_00317#0002</v>
       </c>
       <c r="H10" s="188" t="str">
         <f>_xll.ohRangeRetrieveError(G10)</f>
@@ -13456,7 +13486,7 @@
       </c>
       <c r="G11" s="187" t="str">
         <f>_xll.qlFraRateHelper(,F11,B11,E11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0031a#0000</v>
+        <v>obj_0031c#0002</v>
       </c>
       <c r="H11" s="188" t="str">
         <f>_xll.ohRangeRetrieveError(G11)</f>
@@ -13487,7 +13517,7 @@
       </c>
       <c r="G12" s="187" t="str">
         <f>_xll.qlFraRateHelper(,F12,B12,E12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00315#0000</v>
+        <v>obj_00322#0002</v>
       </c>
       <c r="H12" s="188" t="str">
         <f>_xll.ohRangeRetrieveError(G12)</f>
@@ -13518,7 +13548,7 @@
       </c>
       <c r="G13" s="187" t="str">
         <f>_xll.qlFraRateHelper(,F13,B13,E13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00319#0000</v>
+        <v>obj_0031a#0002</v>
       </c>
       <c r="H13" s="188" t="str">
         <f>_xll.ohRangeRetrieveError(G13)</f>
@@ -13629,7 +13659,7 @@
       </c>
       <c r="D3" s="156" t="str">
         <f t="array" ref="D3:D44">_xll.qlIMMNextCodes(_xll.qlSettingsEvaluationDate(Trigger)-1,$C3:$C44)</f>
-        <v>F5</v>
+        <v>G5</v>
       </c>
       <c r="E3" s="156" t="str">
         <f t="shared" ref="E3:E34" si="0">PROPER(Currency)&amp;FamilyName&amp;$E$1</f>
@@ -13637,15 +13667,15 @@
       </c>
       <c r="F3" s="157" t="str">
         <f t="shared" ref="F3:F34" si="1">Currency&amp;"FUT"&amp;$E$1&amp;$D3&amp;QuoteSuffix</f>
-        <v>JPYFUT3MF5_Quote</v>
+        <v>JPYFUT3MG5_Quote</v>
       </c>
       <c r="G3" s="157" t="str">
         <f t="shared" ref="G3:G34" si="2">Currency&amp;"FUT"&amp;$E$1&amp;$D3&amp;"ConvAdj"&amp;QuoteSuffix</f>
-        <v>JPYFUT3MF5ConvAdj_Quote</v>
+        <v>JPYFUT3MG5ConvAdj_Quote</v>
       </c>
       <c r="H3" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(,$F3,$D3,$E3,$G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00342#0000</v>
+        <v>obj_0036e#0002</v>
       </c>
       <c r="I3" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -13663,7 +13693,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="160" t="str">
-        <v>G5</v>
+        <v>H5</v>
       </c>
       <c r="E4" s="156" t="str">
         <f t="shared" si="0"/>
@@ -13671,15 +13701,15 @@
       </c>
       <c r="F4" s="157" t="str">
         <f t="shared" si="1"/>
-        <v>JPYFUT3MG5_Quote</v>
+        <v>JPYFUT3MH5_Quote</v>
       </c>
       <c r="G4" s="157" t="str">
         <f t="shared" si="2"/>
-        <v>JPYFUT3MG5ConvAdj_Quote</v>
+        <v>JPYFUT3MH5ConvAdj_Quote</v>
       </c>
       <c r="H4" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F4,$D4,$E4,$G4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00365#0000</v>
+        <v>obj_00360#0002</v>
       </c>
       <c r="I4" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -13697,7 +13727,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="160" t="str">
-        <v>H5</v>
+        <v>J5</v>
       </c>
       <c r="E5" s="156" t="str">
         <f t="shared" si="0"/>
@@ -13705,15 +13735,15 @@
       </c>
       <c r="F5" s="157" t="str">
         <f t="shared" si="1"/>
-        <v>JPYFUT3MH5_Quote</v>
+        <v>JPYFUT3MJ5_Quote</v>
       </c>
       <c r="G5" s="157" t="str">
         <f t="shared" si="2"/>
-        <v>JPYFUT3MH5ConvAdj_Quote</v>
+        <v>JPYFUT3MJ5ConvAdj_Quote</v>
       </c>
       <c r="H5" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F5,$D5,$E5,$G5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035d#0000</v>
+        <v>obj_0036b#0002</v>
       </c>
       <c r="I5" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -13731,7 +13761,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="160" t="str">
-        <v>J5</v>
+        <v>K5</v>
       </c>
       <c r="E6" s="156" t="str">
         <f t="shared" si="0"/>
@@ -13739,15 +13769,15 @@
       </c>
       <c r="F6" s="157" t="str">
         <f t="shared" si="1"/>
-        <v>JPYFUT3MJ5_Quote</v>
+        <v>JPYFUT3MK5_Quote</v>
       </c>
       <c r="G6" s="157" t="str">
         <f t="shared" si="2"/>
-        <v>JPYFUT3MJ5ConvAdj_Quote</v>
+        <v>JPYFUT3MK5ConvAdj_Quote</v>
       </c>
       <c r="H6" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F6,$D6,$E6,$G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035c#0000</v>
+        <v>obj_00376#0002</v>
       </c>
       <c r="I6" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -13765,7 +13795,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="160" t="str">
-        <v>K5</v>
+        <v>M5</v>
       </c>
       <c r="E7" s="156" t="str">
         <f t="shared" si="0"/>
@@ -13773,15 +13803,15 @@
       </c>
       <c r="F7" s="157" t="str">
         <f t="shared" si="1"/>
-        <v>JPYFUT3MK5_Quote</v>
+        <v>JPYFUT3MM5_Quote</v>
       </c>
       <c r="G7" s="157" t="str">
         <f t="shared" si="2"/>
-        <v>JPYFUT3MK5ConvAdj_Quote</v>
+        <v>JPYFUT3MM5ConvAdj_Quote</v>
       </c>
       <c r="H7" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F7,$D7,$E7,$G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0036d#0000</v>
+        <v>obj_00359#0002</v>
       </c>
       <c r="I7" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -13799,7 +13829,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="160" t="str">
-        <v>M5</v>
+        <v>N5</v>
       </c>
       <c r="E8" s="156" t="str">
         <f t="shared" si="0"/>
@@ -13807,15 +13837,15 @@
       </c>
       <c r="F8" s="157" t="str">
         <f t="shared" si="1"/>
-        <v>JPYFUT3MM5_Quote</v>
+        <v>JPYFUT3MN5_Quote</v>
       </c>
       <c r="G8" s="157" t="str">
         <f t="shared" si="2"/>
-        <v>JPYFUT3MM5ConvAdj_Quote</v>
+        <v>JPYFUT3MN5ConvAdj_Quote</v>
       </c>
       <c r="H8" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F8,$D8,$E8,$G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00348#0000</v>
+        <v>obj_00356#0002</v>
       </c>
       <c r="I8" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -13833,7 +13863,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="160" t="str">
-        <v>N5</v>
+        <v>Q5</v>
       </c>
       <c r="E9" s="156" t="str">
         <f t="shared" si="0"/>
@@ -13841,15 +13871,15 @@
       </c>
       <c r="F9" s="157" t="str">
         <f t="shared" si="1"/>
-        <v>JPYFUT3MN5_Quote</v>
+        <v>JPYFUT3MQ5_Quote</v>
       </c>
       <c r="G9" s="157" t="str">
         <f t="shared" si="2"/>
-        <v>JPYFUT3MN5ConvAdj_Quote</v>
+        <v>JPYFUT3MQ5ConvAdj_Quote</v>
       </c>
       <c r="H9" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F9,$D9,$E9,$G9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00355#0000</v>
+        <v>obj_00372#0002</v>
       </c>
       <c r="I9" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -13867,7 +13897,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="160" t="str">
-        <v>Q5</v>
+        <v>U5</v>
       </c>
       <c r="E10" s="156" t="str">
         <f t="shared" si="0"/>
@@ -13875,15 +13905,15 @@
       </c>
       <c r="F10" s="157" t="str">
         <f t="shared" si="1"/>
-        <v>JPYFUT3MQ5_Quote</v>
+        <v>JPYFUT3MU5_Quote</v>
       </c>
       <c r="G10" s="157" t="str">
         <f t="shared" si="2"/>
-        <v>JPYFUT3MQ5ConvAdj_Quote</v>
+        <v>JPYFUT3MU5ConvAdj_Quote</v>
       </c>
       <c r="H10" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F10,$D10,$E10,$G10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00360#0000</v>
+        <v>obj_00358#0002</v>
       </c>
       <c r="I10" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -13901,7 +13931,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="160" t="str">
-        <v>U5</v>
+        <v>V5</v>
       </c>
       <c r="E11" s="156" t="str">
         <f t="shared" si="0"/>
@@ -13909,15 +13939,15 @@
       </c>
       <c r="F11" s="157" t="str">
         <f t="shared" si="1"/>
-        <v>JPYFUT3MU5_Quote</v>
+        <v>JPYFUT3MV5_Quote</v>
       </c>
       <c r="G11" s="157" t="str">
         <f t="shared" si="2"/>
-        <v>JPYFUT3MU5ConvAdj_Quote</v>
+        <v>JPYFUT3MV5ConvAdj_Quote</v>
       </c>
       <c r="H11" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F11,$D11,$E11,$G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00376#0000</v>
+        <v>obj_0036c#0002</v>
       </c>
       <c r="I11" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H11)</f>
@@ -13935,7 +13965,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="160" t="str">
-        <v>V5</v>
+        <v>X5</v>
       </c>
       <c r="E12" s="156" t="str">
         <f t="shared" si="0"/>
@@ -13943,15 +13973,15 @@
       </c>
       <c r="F12" s="157" t="str">
         <f t="shared" si="1"/>
-        <v>JPYFUT3MV5_Quote</v>
+        <v>JPYFUT3MX5_Quote</v>
       </c>
       <c r="G12" s="157" t="str">
         <f t="shared" si="2"/>
-        <v>JPYFUT3MV5ConvAdj_Quote</v>
+        <v>JPYFUT3MX5ConvAdj_Quote</v>
       </c>
       <c r="H12" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F12,$D12,$E12,$G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00332#0000</v>
+        <v>obj_00364#0002</v>
       </c>
       <c r="I12" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H12)</f>
@@ -13969,7 +13999,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="160" t="str">
-        <v>X5</v>
+        <v>Z5</v>
       </c>
       <c r="E13" s="156" t="str">
         <f t="shared" si="0"/>
@@ -13977,15 +14007,15 @@
       </c>
       <c r="F13" s="157" t="str">
         <f t="shared" si="1"/>
-        <v>JPYFUT3MX5_Quote</v>
+        <v>JPYFUT3MZ5_Quote</v>
       </c>
       <c r="G13" s="157" t="str">
         <f t="shared" si="2"/>
-        <v>JPYFUT3MX5ConvAdj_Quote</v>
+        <v>JPYFUT3MZ5ConvAdj_Quote</v>
       </c>
       <c r="H13" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F13,$D13,$E13,$G13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00346#0000</v>
+        <v>obj_0036a#0002</v>
       </c>
       <c r="I13" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H13)</f>
@@ -14003,7 +14033,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="160" t="str">
-        <v>Z5</v>
+        <v>F6</v>
       </c>
       <c r="E14" s="156" t="str">
         <f t="shared" si="0"/>
@@ -14011,15 +14041,15 @@
       </c>
       <c r="F14" s="157" t="str">
         <f t="shared" si="1"/>
-        <v>JPYFUT3MZ5_Quote</v>
+        <v>JPYFUT3MF6_Quote</v>
       </c>
       <c r="G14" s="157" t="str">
         <f t="shared" si="2"/>
-        <v>JPYFUT3MZ5ConvAdj_Quote</v>
+        <v>JPYFUT3MF6ConvAdj_Quote</v>
       </c>
       <c r="H14" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F14,$D14,$E14,$G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034a#0000</v>
+        <v>obj_0035f#0002</v>
       </c>
       <c r="I14" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H14)</f>
@@ -14053,7 +14083,7 @@
       </c>
       <c r="H15" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F15,$D15,$E15,$G15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00331#0000</v>
+        <v>obj_00361#0002</v>
       </c>
       <c r="I15" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H15)</f>
@@ -14087,7 +14117,7 @@
       </c>
       <c r="H16" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F16,$D16,$E16,$G16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00340#0000</v>
+        <v>obj_0035b#0002</v>
       </c>
       <c r="I16" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H16)</f>
@@ -14121,7 +14151,7 @@
       </c>
       <c r="H17" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F17,$D17,$E17,$G17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0032f#0000</v>
+        <v>obj_0035e#0002</v>
       </c>
       <c r="I17" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H17)</f>
@@ -14155,7 +14185,7 @@
       </c>
       <c r="H18" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F18,$D18,$E18,$G18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00344#0000</v>
+        <v>obj_00374#0002</v>
       </c>
       <c r="I18" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H18)</f>
@@ -14189,7 +14219,7 @@
       </c>
       <c r="H19" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F19,$D19,$E19,$G19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00349#0000</v>
+        <v>obj_0035c#0002</v>
       </c>
       <c r="I19" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H19)</f>
@@ -14223,7 +14253,7 @@
       </c>
       <c r="H20" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F20,$D20,$E20,$G20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00378#0000</v>
+        <v>obj_0035a#0002</v>
       </c>
       <c r="I20" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H20)</f>
@@ -14257,7 +14287,7 @@
       </c>
       <c r="H21" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F21,$D21,$E21,$G21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00377#0000</v>
+        <v>obj_00354#0002</v>
       </c>
       <c r="I21" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H21)</f>
@@ -14291,7 +14321,7 @@
       </c>
       <c r="H22" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F22,$D22,$E22,$G22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0033f#0000</v>
+        <v>obj_00355#0002</v>
       </c>
       <c r="I22" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H22)</f>
@@ -14325,7 +14355,7 @@
       </c>
       <c r="H23" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F23,$D23,$E23,$G23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035e#0000</v>
+        <v>obj_00352#0002</v>
       </c>
       <c r="I23" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H23)</f>
@@ -14359,7 +14389,7 @@
       </c>
       <c r="H24" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F24,$D24,$E24,$G24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00368#0000</v>
+        <v>obj_00366#0002</v>
       </c>
       <c r="I24" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H24)</f>
@@ -14393,7 +14423,7 @@
       </c>
       <c r="H25" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F25,$D25,$E25,$G25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00351#0000</v>
+        <v>obj_00377#0002</v>
       </c>
       <c r="I25" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H25)</f>
@@ -14427,7 +14457,7 @@
       </c>
       <c r="H26" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F26,$D26,$E26,$G26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00336#0000</v>
+        <v>obj_00375#0002</v>
       </c>
       <c r="I26" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H26)</f>
@@ -14461,7 +14491,7 @@
       </c>
       <c r="H27" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F27,$D27,$E27,$G27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00362#0000</v>
+        <v>obj_0036d#0002</v>
       </c>
       <c r="I27" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H27)</f>
@@ -14495,7 +14525,7 @@
       </c>
       <c r="H28" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F28,$D28,$E28,$G28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034e#0000</v>
+        <v>obj_00365#0002</v>
       </c>
       <c r="I28" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H28)</f>
@@ -14529,7 +14559,7 @@
       </c>
       <c r="H29" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F29,$D29,$E29,$G29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034c#0000</v>
+        <v>obj_00362#0002</v>
       </c>
       <c r="I29" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H29)</f>
@@ -14563,7 +14593,7 @@
       </c>
       <c r="H30" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F30,$D30,$E30,$G30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00374#0000</v>
+        <v>obj_00367#0002</v>
       </c>
       <c r="I30" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H30)</f>
@@ -14597,7 +14627,7 @@
       </c>
       <c r="H31" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F31,$D31,$E31,$G31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0033a#0000</v>
+        <v>obj_0034f#0002</v>
       </c>
       <c r="I31" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H31)</f>
@@ -14631,7 +14661,7 @@
       </c>
       <c r="H32" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F32,$D32,$E32,$G32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00345#0000</v>
+        <v>obj_00368#0002</v>
       </c>
       <c r="I32" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H32)</f>
@@ -14665,7 +14695,7 @@
       </c>
       <c r="H33" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F33,$D33,$E33,$G33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0036f#0000</v>
+        <v>obj_00370#0002</v>
       </c>
       <c r="I33" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H33)</f>
@@ -14699,7 +14729,7 @@
       </c>
       <c r="H34" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F34,$D34,$E34,$G34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00353#0000</v>
+        <v>obj_00357#0002</v>
       </c>
       <c r="I34" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H34)</f>
@@ -14733,7 +14763,7 @@
       </c>
       <c r="H35" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F35,$D35,$E35,$G35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00354#0000</v>
+        <v>obj_0036f#0002</v>
       </c>
       <c r="I35" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H35)</f>
@@ -14767,7 +14797,7 @@
       </c>
       <c r="H36" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F36,$D36,$E36,$G36,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0036c#0000</v>
+        <v>obj_00353#0002</v>
       </c>
       <c r="I36" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H36)</f>
@@ -14801,7 +14831,7 @@
       </c>
       <c r="H37" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F37,$D37,$E37,$G37,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00375#0000</v>
+        <v>obj_00369#0002</v>
       </c>
       <c r="I37" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H37)</f>
@@ -14835,7 +14865,7 @@
       </c>
       <c r="H38" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F38,$D38,$E38,$G38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00371#0000</v>
+        <v>obj_00373#0002</v>
       </c>
       <c r="I38" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H38)</f>
@@ -14869,7 +14899,7 @@
       </c>
       <c r="H39" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F39,$D39,$E39,$G39,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00352#0000</v>
+        <v>obj_00351#0002</v>
       </c>
       <c r="I39" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H39)</f>
@@ -14903,7 +14933,7 @@
       </c>
       <c r="H40" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F40,$D40,$E40,$G40,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00343#0000</v>
+        <v>obj_00371#0002</v>
       </c>
       <c r="I40" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H40)</f>
@@ -14936,7 +14966,7 @@
       </c>
       <c r="H41" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F41,$D41,$E41,$G41,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00367#0000</v>
+        <v>obj_00363#0002</v>
       </c>
       <c r="I41" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H41)</f>
@@ -14969,7 +14999,7 @@
       </c>
       <c r="H42" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F42,$D42,$E42,$G42,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00347#0000</v>
+        <v>obj_00350#0002</v>
       </c>
       <c r="I42" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H42)</f>
@@ -15002,7 +15032,7 @@
       </c>
       <c r="H43" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F43,$D43,$E43,$G43,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034f#0000</v>
+        <v>obj_00378#0002</v>
       </c>
       <c r="I43" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H43)</f>
@@ -15035,7 +15065,7 @@
       </c>
       <c r="H44" s="161" t="str">
         <f>_xll.qlFuturesRateHelper(,$F44,$D44,$E44,$G44,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0036e#0000</v>
+        <v>obj_0035d#0002</v>
       </c>
       <c r="I44" s="50" t="str">
         <f>_xll.ohRangeRetrieveError(H44)</f>
@@ -15159,7 +15189,7 @@
       <c r="J3" s="66"/>
       <c r="K3" s="168" t="str">
         <f>_xll.qlLibor(,Currency,$I$1,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00323#0000</v>
+        <v>obj_0031f#0002</v>
       </c>
       <c r="L3" s="169" t="str">
         <f>_xll.ohRangeRetrieveError(K3)</f>
@@ -15217,8 +15247,8 @@
         <v>JPYSB6L1Y_Quote</v>
       </c>
       <c r="K5" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J5,$C5,SwapCalendar,$F5,$G5,$H5,$K$3,$I5,B5,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00329#0008</v>
+        <f>_xll.qlSwapRateHelper2(,$J5,$C5,Calendar,$F5,$G5,$H5,$K$3,$I5,B5,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00339#0003</v>
       </c>
       <c r="L5" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K5)</f>
@@ -15264,8 +15294,8 @@
         <v>JPYSB6L15M_Quote</v>
       </c>
       <c r="K6" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J6,$C6,SwapCalendar,$F6,$G6,$H6,$K$3,$I6,B6,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0032e#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J6,$C6,Calendar,$F6,$G6,$H6,$K$3,$I6,B6,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0033e#0003</v>
       </c>
       <c r="L6" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K6)</f>
@@ -15315,8 +15345,8 @@
         <v>JPYSB6L18M_Quote</v>
       </c>
       <c r="K7" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J7,$C7,SwapCalendar,$F7,$G7,$H7,$K$3,$I7,B7,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00370#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J7,$C7,Calendar,$F7,$G7,$H7,$K$3,$I7,B7,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0032c#0003</v>
       </c>
       <c r="L7" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K7)</f>
@@ -15366,8 +15396,8 @@
         <v>JPYSB6L21M_Quote</v>
       </c>
       <c r="K8" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J8,$C8,SwapCalendar,$F8,$G8,$H8,$K$3,$I8,B8,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0032d#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J8,$C8,Calendar,$F8,$G8,$H8,$K$3,$I8,B8,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00338#0003</v>
       </c>
       <c r="L8" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K8)</f>
@@ -15417,8 +15447,8 @@
         <v>JPYSB6L2Y_Quote</v>
       </c>
       <c r="K9" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J9,$C9,SwapCalendar,$F9,$G9,$H9,$K$3,$I9,B9,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00330#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J9,$C9,Calendar,$F9,$G9,$H9,$K$3,$I9,B9,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00346#0003</v>
       </c>
       <c r="L9" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K9)</f>
@@ -15468,8 +15498,8 @@
         <v>JPYSB6L3Y_Quote</v>
       </c>
       <c r="K10" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J10,$C10,SwapCalendar,$F10,$G10,$H10,$K$3,$I10,B10,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00361#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J10,$C10,Calendar,$F10,$G10,$H10,$K$3,$I10,B10,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0032f#0003</v>
       </c>
       <c r="L10" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K10)</f>
@@ -15510,8 +15540,8 @@
         <v>JPYSB6L4Y_Quote</v>
       </c>
       <c r="K11" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J11,$C11,SwapCalendar,$F11,$G11,$H11,$K$3,$I11,B11,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00358#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J11,$C11,Calendar,$F11,$G11,$H11,$K$3,$I11,B11,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00340#0003</v>
       </c>
       <c r="L11" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K11)</f>
@@ -15552,8 +15582,8 @@
         <v>JPYSB6L5Y_Quote</v>
       </c>
       <c r="K12" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J12,$C12,SwapCalendar,$F12,$G12,$H12,$K$3,$I12,B12,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00373#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J12,$C12,Calendar,$F12,$G12,$H12,$K$3,$I12,B12,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0032e#0003</v>
       </c>
       <c r="L12" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K12)</f>
@@ -15594,8 +15624,8 @@
         <v>JPYSB6L6Y_Quote</v>
       </c>
       <c r="K13" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J13,$C13,SwapCalendar,$F13,$G13,$H13,$K$3,$I13,B13,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00359#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J13,$C13,Calendar,$F13,$G13,$H13,$K$3,$I13,B13,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0033f#0003</v>
       </c>
       <c r="L13" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K13)</f>
@@ -15636,8 +15666,8 @@
         <v>JPYSB6L7Y_Quote</v>
       </c>
       <c r="K14" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J14,$C14,SwapCalendar,$F14,$G14,$H14,$K$3,$I14,B14,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00363#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J14,$C14,Calendar,$F14,$G14,$H14,$K$3,$I14,B14,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00331#0003</v>
       </c>
       <c r="L14" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K14)</f>
@@ -15678,8 +15708,8 @@
         <v>JPYSB6L8Y_Quote</v>
       </c>
       <c r="K15" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J15,$C15,SwapCalendar,$F15,$G15,$H15,$K$3,$I15,B15,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0035f#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J15,$C15,Calendar,$F15,$G15,$H15,$K$3,$I15,B15,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0034c#0003</v>
       </c>
       <c r="L15" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K15)</f>
@@ -15720,8 +15750,8 @@
         <v>JPYSB6L9Y_Quote</v>
       </c>
       <c r="K16" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J16,$C16,SwapCalendar,$F16,$G16,$H16,$K$3,$I16,B16,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0033e#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J16,$C16,Calendar,$F16,$G16,$H16,$K$3,$I16,B16,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00334#0003</v>
       </c>
       <c r="L16" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K16)</f>
@@ -15762,8 +15792,8 @@
         <v>JPYSB6L10Y_Quote</v>
       </c>
       <c r="K17" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J17,$C17,SwapCalendar,$F17,$G17,$H17,$K$3,$I17,B17,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00372#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J17,$C17,Calendar,$F17,$G17,$H17,$K$3,$I17,B17,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00341#0003</v>
       </c>
       <c r="L17" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K17)</f>
@@ -15804,8 +15834,8 @@
         <v>JPYSB6L11Y_Quote</v>
       </c>
       <c r="K18" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J18,$C18,SwapCalendar,$F18,$G18,$H18,$K$3,$I18,B18,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0033c#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J18,$C18,Calendar,$F18,$G18,$H18,$K$3,$I18,B18,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0032a#0003</v>
       </c>
       <c r="L18" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K18)</f>
@@ -15846,8 +15876,8 @@
         <v>JPYSB6L12Y_Quote</v>
       </c>
       <c r="K19" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J19,$C19,SwapCalendar,$F19,$G19,$H19,$K$3,$I19,B19,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0034d#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J19,$C19,Calendar,$F19,$G19,$H19,$K$3,$I19,B19,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0033b#0003</v>
       </c>
       <c r="L19" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K19)</f>
@@ -15888,8 +15918,8 @@
         <v>JPYSB6L13Y_Quote</v>
       </c>
       <c r="K20" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J20,$C20,SwapCalendar,$F20,$G20,$H20,$K$3,$I20,B20,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0036a#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J20,$C20,Calendar,$F20,$G20,$H20,$K$3,$I20,B20,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00329#0003</v>
       </c>
       <c r="L20" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K20)</f>
@@ -15930,8 +15960,8 @@
         <v>JPYSB6L14Y_Quote</v>
       </c>
       <c r="K21" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J21,$C21,SwapCalendar,$F21,$G21,$H21,$K$3,$I21,B21,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0035b#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J21,$C21,Calendar,$F21,$G21,$H21,$K$3,$I21,B21,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0033a#0003</v>
       </c>
       <c r="L21" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K21)</f>
@@ -15972,8 +16002,8 @@
         <v>JPYSB6L15Y_Quote</v>
       </c>
       <c r="K22" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J22,$C22,SwapCalendar,$F22,$G22,$H22,$K$3,$I22,B22,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0034b#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J22,$C22,Calendar,$F22,$G22,$H22,$K$3,$I22,B22,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0032d#0003</v>
       </c>
       <c r="L22" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K22)</f>
@@ -16014,8 +16044,8 @@
         <v>JPYSB6L16Y_Quote</v>
       </c>
       <c r="K23" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J23,$C23,SwapCalendar,$F23,$G23,$H23,$K$3,$I23,B23,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00339#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J23,$C23,Calendar,$F23,$G23,$H23,$K$3,$I23,B23,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00347#0003</v>
       </c>
       <c r="L23" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K23)</f>
@@ -16056,8 +16086,8 @@
         <v>JPYSB6L17Y_Quote</v>
       </c>
       <c r="K24" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J24,$C24,SwapCalendar,$F24,$G24,$H24,$K$3,$I24,B24,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0033b#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J24,$C24,Calendar,$F24,$G24,$H24,$K$3,$I24,B24,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00330#0003</v>
       </c>
       <c r="L24" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K24)</f>
@@ -16098,8 +16128,8 @@
         <v>JPYSB6L18Y_Quote</v>
       </c>
       <c r="K25" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J25,$C25,SwapCalendar,$F25,$G25,$H25,$K$3,$I25,B25,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00335#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J25,$C25,Calendar,$F25,$G25,$H25,$K$3,$I25,B25,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0033c#0003</v>
       </c>
       <c r="L25" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K25)</f>
@@ -16140,8 +16170,8 @@
         <v>JPYSB6L19Y_Quote</v>
       </c>
       <c r="K26" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J26,$C26,SwapCalendar,$F26,$G26,$H26,$K$3,$I26,B26,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0035a#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J26,$C26,Calendar,$F26,$G26,$H26,$K$3,$I26,B26,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0034a#0003</v>
       </c>
       <c r="L26" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K26)</f>
@@ -16182,8 +16212,8 @@
         <v>JPYSB6L20Y_Quote</v>
       </c>
       <c r="K27" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J27,$C27,SwapCalendar,$F27,$G27,$H27,$K$3,$I27,B27,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00356#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J27,$C27,Calendar,$F27,$G27,$H27,$K$3,$I27,B27,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00336#0003</v>
       </c>
       <c r="L27" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K27)</f>
@@ -16224,8 +16254,8 @@
         <v>JPYSB6L21Y_Quote</v>
       </c>
       <c r="K28" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J28,$C28,SwapCalendar,$F28,$G28,$H28,$K$3,$I28,B28,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0036b#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J28,$C28,Calendar,$F28,$G28,$H28,$K$3,$I28,B28,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00349#0003</v>
       </c>
       <c r="L28" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K28)</f>
@@ -16266,8 +16296,8 @@
         <v>JPYSB6L22Y_Quote</v>
       </c>
       <c r="K29" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J29,$C29,SwapCalendar,$F29,$G29,$H29,$K$3,$I29,B29,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00350#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J29,$C29,Calendar,$F29,$G29,$H29,$K$3,$I29,B29,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00335#0003</v>
       </c>
       <c r="L29" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K29)</f>
@@ -16308,8 +16338,8 @@
         <v>JPYSB6L23Y_Quote</v>
       </c>
       <c r="K30" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J30,$C30,SwapCalendar,$F30,$G30,$H30,$K$3,$I30,B30,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0032b#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J30,$C30,Calendar,$F30,$G30,$H30,$K$3,$I30,B30,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00328#0003</v>
       </c>
       <c r="L30" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K30)</f>
@@ -16350,8 +16380,8 @@
         <v>JPYSB6L24Y_Quote</v>
       </c>
       <c r="K31" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J31,$C31,SwapCalendar,$F31,$G31,$H31,$K$3,$I31,B31,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00334#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J31,$C31,Calendar,$F31,$G31,$H31,$K$3,$I31,B31,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00342#0003</v>
       </c>
       <c r="L31" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K31)</f>
@@ -16392,8 +16422,8 @@
         <v>JPYSB6L25Y_Quote</v>
       </c>
       <c r="K32" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J32,$C32,SwapCalendar,$F32,$G32,$H32,$K$3,$I32,B32,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00357#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J32,$C32,Calendar,$F32,$G32,$H32,$K$3,$I32,B32,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0032b#0003</v>
       </c>
       <c r="L32" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K32)</f>
@@ -16434,8 +16464,8 @@
         <v>JPYSB6L26Y_Quote</v>
       </c>
       <c r="K33" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J33,$C33,SwapCalendar,$F33,$G33,$H33,$K$3,$I33,B33,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00364#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J33,$C33,Calendar,$F33,$G33,$H33,$K$3,$I33,B33,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00337#0003</v>
       </c>
       <c r="L33" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K33)</f>
@@ -16476,8 +16506,8 @@
         <v>JPYSB6L27Y_Quote</v>
       </c>
       <c r="K34" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J34,$C34,SwapCalendar,$F34,$G34,$H34,$K$3,$I34,B34,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00369#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J34,$C34,Calendar,$F34,$G34,$H34,$K$3,$I34,B34,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00345#0003</v>
       </c>
       <c r="L34" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K34)</f>
@@ -16518,8 +16548,8 @@
         <v>JPYSB6L28Y_Quote</v>
       </c>
       <c r="K35" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J35,$C35,SwapCalendar,$F35,$G35,$H35,$K$3,$I35,B35,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00338#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J35,$C35,Calendar,$F35,$G35,$H35,$K$3,$I35,B35,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00332#0003</v>
       </c>
       <c r="L35" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K35)</f>
@@ -16560,8 +16590,8 @@
         <v>JPYSB6L29Y_Quote</v>
       </c>
       <c r="K36" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J36,$C36,SwapCalendar,$F36,$G36,$H36,$K$3,$I36,B36,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0032c#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J36,$C36,Calendar,$F36,$G36,$H36,$K$3,$I36,B36,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00344#0003</v>
       </c>
       <c r="L36" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K36)</f>
@@ -16602,8 +16632,8 @@
         <v>JPYSB6L30Y_Quote</v>
       </c>
       <c r="K37" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J37,$C37,SwapCalendar,$F37,$G37,$H37,$K$3,$I37,B37,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00341#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J37,$C37,Calendar,$F37,$G37,$H37,$K$3,$I37,B37,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00343#0003</v>
       </c>
       <c r="L37" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K37)</f>
@@ -16644,8 +16674,8 @@
         <v>JPYSB6L35Y_Quote</v>
       </c>
       <c r="K38" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J38,$C38,SwapCalendar,$F38,$G38,$H38,$K$3,$I38,B38,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0033d#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J38,$C38,Calendar,$F38,$G38,$H38,$K$3,$I38,B38,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00348#0003</v>
       </c>
       <c r="L38" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K38)</f>
@@ -16686,8 +16716,8 @@
         <v>JPYSB6L40Y_Quote</v>
       </c>
       <c r="K39" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J39,$C39,SwapCalendar,$F39,$G39,$H39,$K$3,$I39,B39,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00337#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J39,$C39,Calendar,$F39,$G39,$H39,$K$3,$I39,B39,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0033d#0003</v>
       </c>
       <c r="L39" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K39)</f>
@@ -16728,8 +16758,8 @@
         <v>JPYSB6L50Y_Quote</v>
       </c>
       <c r="K40" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J40,$C40,SwapCalendar,$F40,$G40,$H40,$K$3,$I40,B40,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00333#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J40,$C40,Calendar,$F40,$G40,$H40,$K$3,$I40,B40,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0034b#0003</v>
       </c>
       <c r="L40" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K40)</f>
@@ -16770,8 +16800,8 @@
         <v>JPYSB6L60Y_Quote</v>
       </c>
       <c r="K41" s="173" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J41,$C41,SwapCalendar,$F41,$G41,$H41,$K$3,$I41,B41,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00366#0002</v>
+        <f>_xll.qlSwapRateHelper2(,$J41,$C41,Calendar,$F41,$G41,$H41,$K$3,$I41,B41,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00333#0003</v>
       </c>
       <c r="L41" s="166" t="str">
         <f>_xll.ohRangeRetrieveError(K41)</f>

</xml_diff>